<commit_message>
fix:delete sd and ed
</commit_message>
<xml_diff>
--- a/xlsx_template/data_template.xlsx
+++ b/xlsx_template/data_template.xlsx
@@ -3400,7 +3400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3698,16 +3698,34 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3722,32 +3740,8 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3755,19 +3749,31 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3779,13 +3785,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3793,15 +3793,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3811,21 +3802,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3842,7 +3818,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3851,21 +3833,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3889,6 +3880,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3931,7 +3934,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5997,19 +6000,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="29.25" customHeight="1">
-      <c r="B2" s="172" t="s">
+      <c r="B2" s="170" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="199" t="s">
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="193" t="s">
         <v>282</v>
       </c>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
       <c r="K2" s="116"/>
       <c r="L2" s="116"/>
       <c r="N2" s="78" t="s">
@@ -6017,86 +6020,86 @@
       </c>
     </row>
     <row r="4" spans="2:14" ht="15.75" thickBot="1">
-      <c r="K4" s="202" t="s">
+      <c r="K4" s="211" t="s">
         <v>473</v>
       </c>
-      <c r="L4" s="202"/>
-      <c r="M4" s="202"/>
+      <c r="L4" s="211"/>
+      <c r="M4" s="211"/>
     </row>
     <row r="5" spans="2:14" ht="15.75" thickTop="1">
-      <c r="B5" s="208" t="s">
+      <c r="B5" s="205" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="210" t="s">
+      <c r="C5" s="207" t="s">
         <v>262</v>
       </c>
-      <c r="D5" s="196" t="s">
+      <c r="D5" s="188" t="s">
         <v>263</v>
       </c>
-      <c r="E5" s="212" t="s">
+      <c r="E5" s="209" t="s">
         <v>264</v>
       </c>
-      <c r="F5" s="212"/>
-      <c r="G5" s="212" t="s">
+      <c r="F5" s="209"/>
+      <c r="G5" s="209" t="s">
         <v>267</v>
       </c>
-      <c r="H5" s="212"/>
-      <c r="I5" s="212"/>
-      <c r="J5" s="212"/>
-      <c r="K5" s="212" t="s">
+      <c r="H5" s="209"/>
+      <c r="I5" s="209"/>
+      <c r="J5" s="209"/>
+      <c r="K5" s="209" t="s">
         <v>272</v>
       </c>
-      <c r="L5" s="212"/>
-      <c r="M5" s="212"/>
-      <c r="N5" s="213"/>
+      <c r="L5" s="209"/>
+      <c r="M5" s="209"/>
+      <c r="N5" s="210"/>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="209"/>
-      <c r="C6" s="211"/>
-      <c r="D6" s="190"/>
-      <c r="E6" s="206" t="s">
+      <c r="B6" s="206"/>
+      <c r="C6" s="208"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="203" t="s">
         <v>265</v>
       </c>
-      <c r="F6" s="206" t="s">
+      <c r="F6" s="203" t="s">
         <v>266</v>
       </c>
-      <c r="G6" s="206" t="s">
+      <c r="G6" s="203" t="s">
         <v>268</v>
       </c>
-      <c r="H6" s="206" t="s">
+      <c r="H6" s="203" t="s">
         <v>269</v>
       </c>
-      <c r="I6" s="206" t="s">
+      <c r="I6" s="203" t="s">
         <v>270</v>
       </c>
-      <c r="J6" s="206"/>
-      <c r="K6" s="206" t="s">
+      <c r="J6" s="203"/>
+      <c r="K6" s="203" t="s">
         <v>273</v>
       </c>
-      <c r="L6" s="206" t="s">
+      <c r="L6" s="203" t="s">
         <v>269</v>
       </c>
-      <c r="M6" s="206" t="s">
+      <c r="M6" s="203" t="s">
         <v>270</v>
       </c>
-      <c r="N6" s="207"/>
+      <c r="N6" s="204"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="209"/>
-      <c r="C7" s="211"/>
-      <c r="D7" s="190"/>
-      <c r="E7" s="206"/>
-      <c r="F7" s="206"/>
-      <c r="G7" s="206"/>
-      <c r="H7" s="206"/>
+      <c r="B7" s="206"/>
+      <c r="C7" s="208"/>
+      <c r="D7" s="189"/>
+      <c r="E7" s="203"/>
+      <c r="F7" s="203"/>
+      <c r="G7" s="203"/>
+      <c r="H7" s="203"/>
       <c r="I7" s="86" t="s">
         <v>271</v>
       </c>
       <c r="J7" s="86" t="s">
         <v>141</v>
       </c>
-      <c r="K7" s="206"/>
-      <c r="L7" s="206"/>
+      <c r="K7" s="203"/>
+      <c r="L7" s="203"/>
       <c r="M7" s="86" t="s">
         <v>122</v>
       </c>
@@ -11848,11 +11851,11 @@
       <c r="H155" s="10"/>
       <c r="I155" s="10"/>
       <c r="J155" s="10"/>
-      <c r="K155" s="205" t="s">
+      <c r="K155" s="214" t="s">
         <v>318</v>
       </c>
-      <c r="L155" s="205"/>
-      <c r="M155" s="205"/>
+      <c r="L155" s="214"/>
+      <c r="M155" s="214"/>
       <c r="N155" s="10"/>
     </row>
     <row r="156" spans="1:14" s="21" customFormat="1" ht="74.25" customHeight="1">
@@ -11862,15 +11865,15 @@
       <c r="D156" s="22"/>
       <c r="E156" s="22"/>
       <c r="F156" s="22"/>
-      <c r="G156" s="203"/>
-      <c r="H156" s="203"/>
-      <c r="I156" s="203"/>
+      <c r="G156" s="212"/>
+      <c r="H156" s="212"/>
+      <c r="I156" s="212"/>
       <c r="J156" s="22"/>
-      <c r="K156" s="204" t="s">
+      <c r="K156" s="213" t="s">
         <v>311</v>
       </c>
-      <c r="L156" s="204"/>
-      <c r="M156" s="204"/>
+      <c r="L156" s="213"/>
+      <c r="M156" s="213"/>
       <c r="N156" s="22"/>
     </row>
     <row r="157" spans="1:14" s="21" customFormat="1" ht="14.25">
@@ -11882,11 +11885,11 @@
       <c r="D157" s="22"/>
       <c r="E157" s="22"/>
       <c r="F157" s="22"/>
-      <c r="G157" s="203" t="s">
+      <c r="G157" s="212" t="s">
         <v>309</v>
       </c>
-      <c r="H157" s="203"/>
-      <c r="I157" s="203"/>
+      <c r="H157" s="212"/>
+      <c r="I157" s="212"/>
       <c r="J157" s="22"/>
       <c r="K157" s="22"/>
       <c r="L157" s="22"/>
@@ -11950,17 +11953,17 @@
       <c r="D161" s="22"/>
       <c r="E161" s="22"/>
       <c r="F161" s="22"/>
-      <c r="G161" s="203" t="s">
+      <c r="G161" s="212" t="s">
         <v>313</v>
       </c>
-      <c r="H161" s="203"/>
-      <c r="I161" s="203"/>
+      <c r="H161" s="212"/>
+      <c r="I161" s="212"/>
       <c r="J161" s="22"/>
-      <c r="K161" s="203" t="s">
+      <c r="K161" s="212" t="s">
         <v>314</v>
       </c>
-      <c r="L161" s="203"/>
-      <c r="M161" s="203"/>
+      <c r="L161" s="212"/>
+      <c r="M161" s="212"/>
       <c r="N161" s="10"/>
     </row>
     <row r="162" spans="1:14">
@@ -12573,6 +12576,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="G156:I156"/>
+    <mergeCell ref="G161:I161"/>
+    <mergeCell ref="K156:M156"/>
+    <mergeCell ref="G157:I157"/>
+    <mergeCell ref="K155:M155"/>
+    <mergeCell ref="K161:M161"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="I6:J6"/>
@@ -12589,13 +12599,6 @@
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="E2:J2"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="G156:I156"/>
-    <mergeCell ref="G161:I161"/>
-    <mergeCell ref="K156:M156"/>
-    <mergeCell ref="G157:I157"/>
-    <mergeCell ref="K155:M155"/>
-    <mergeCell ref="K161:M161"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14888,17 +14891,17 @@
       <c r="C2" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="E2" s="214" t="s">
+      <c r="E2" s="215" t="s">
         <v>307</v>
       </c>
-      <c r="F2" s="214"/>
-      <c r="G2" s="214"/>
-      <c r="H2" s="214"/>
-      <c r="I2" s="214"/>
-      <c r="L2" s="215" t="s">
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
+      <c r="H2" s="215"/>
+      <c r="I2" s="215"/>
+      <c r="L2" s="216" t="s">
         <v>306</v>
       </c>
-      <c r="M2" s="216"/>
+      <c r="M2" s="217"/>
     </row>
     <row r="3" spans="2:13" ht="19.5" customHeight="1">
       <c r="D3" s="131"/>
@@ -14913,30 +14916,30 @@
     </row>
     <row r="4" spans="2:13" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="5" spans="2:13" ht="15.75" thickTop="1">
-      <c r="B5" s="224" t="s">
+      <c r="B5" s="225" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="224" t="s">
         <v>284</v>
       </c>
-      <c r="D5" s="219" t="s">
+      <c r="D5" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="E5" s="219"/>
-      <c r="F5" s="219"/>
-      <c r="G5" s="219"/>
-      <c r="H5" s="219"/>
-      <c r="I5" s="219"/>
-      <c r="J5" s="219"/>
-      <c r="K5" s="219"/>
-      <c r="L5" s="219"/>
-      <c r="M5" s="225" t="s">
+      <c r="E5" s="220"/>
+      <c r="F5" s="220"/>
+      <c r="G5" s="220"/>
+      <c r="H5" s="220"/>
+      <c r="I5" s="220"/>
+      <c r="J5" s="220"/>
+      <c r="K5" s="220"/>
+      <c r="L5" s="220"/>
+      <c r="M5" s="226" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="6" spans="2:13">
-      <c r="B6" s="220"/>
-      <c r="C6" s="221"/>
+      <c r="B6" s="221"/>
+      <c r="C6" s="222"/>
       <c r="D6" s="136" t="s">
         <v>157</v>
       </c>
@@ -14964,21 +14967,21 @@
       <c r="L6" s="137" t="s">
         <v>153</v>
       </c>
-      <c r="M6" s="226"/>
+      <c r="M6" s="227"/>
     </row>
     <row r="7" spans="2:13" ht="10.5" customHeight="1">
-      <c r="B7" s="220"/>
-      <c r="C7" s="221"/>
-      <c r="D7" s="221"/>
-      <c r="E7" s="221"/>
-      <c r="F7" s="221"/>
-      <c r="G7" s="221"/>
-      <c r="H7" s="221"/>
-      <c r="I7" s="221"/>
-      <c r="J7" s="221"/>
-      <c r="K7" s="221"/>
-      <c r="L7" s="221"/>
-      <c r="M7" s="222"/>
+      <c r="B7" s="221"/>
+      <c r="C7" s="222"/>
+      <c r="D7" s="222"/>
+      <c r="E7" s="222"/>
+      <c r="F7" s="222"/>
+      <c r="G7" s="222"/>
+      <c r="H7" s="222"/>
+      <c r="I7" s="222"/>
+      <c r="J7" s="222"/>
+      <c r="K7" s="222"/>
+      <c r="L7" s="222"/>
+      <c r="M7" s="223"/>
     </row>
     <row r="8" spans="2:13" s="3" customFormat="1" ht="14.25">
       <c r="B8" s="27" t="s">
@@ -18634,11 +18637,11 @@
     </row>
     <row r="85" spans="1:14" ht="15.75" thickTop="1">
       <c r="C85" s="18"/>
-      <c r="K85" s="217" t="s">
+      <c r="K85" s="218" t="s">
         <v>310</v>
       </c>
-      <c r="L85" s="217"/>
-      <c r="M85" s="217"/>
+      <c r="L85" s="218"/>
+      <c r="M85" s="218"/>
     </row>
     <row r="86" spans="1:14" ht="61.5" customHeight="1">
       <c r="A86" s="3"/>
@@ -18648,18 +18651,18 @@
       </c>
       <c r="D86" s="130"/>
       <c r="E86" s="130"/>
-      <c r="F86" s="218" t="s">
+      <c r="F86" s="219" t="s">
         <v>309</v>
       </c>
-      <c r="G86" s="218"/>
-      <c r="H86" s="218"/>
+      <c r="G86" s="219"/>
+      <c r="H86" s="219"/>
       <c r="I86" s="130"/>
       <c r="J86" s="130"/>
-      <c r="K86" s="214" t="s">
+      <c r="K86" s="215" t="s">
         <v>311</v>
       </c>
-      <c r="L86" s="214"/>
-      <c r="M86" s="214"/>
+      <c r="L86" s="215"/>
+      <c r="M86" s="215"/>
       <c r="N86" s="3"/>
     </row>
     <row r="87" spans="1:14">
@@ -18702,18 +18705,18 @@
       </c>
       <c r="D89" s="130"/>
       <c r="E89" s="130"/>
-      <c r="F89" s="218" t="s">
+      <c r="F89" s="219" t="s">
         <v>313</v>
       </c>
-      <c r="G89" s="218"/>
-      <c r="H89" s="218"/>
+      <c r="G89" s="219"/>
+      <c r="H89" s="219"/>
       <c r="I89" s="130"/>
       <c r="J89" s="130"/>
-      <c r="K89" s="218" t="s">
+      <c r="K89" s="219" t="s">
         <v>314</v>
       </c>
-      <c r="L89" s="218"/>
-      <c r="M89" s="218"/>
+      <c r="L89" s="219"/>
+      <c r="M89" s="219"/>
       <c r="N89" s="3"/>
     </row>
   </sheetData>
@@ -19041,163 +19044,163 @@
       <c r="F2" s="66"/>
       <c r="G2" s="66"/>
       <c r="H2" s="66"/>
-      <c r="I2" s="161" t="s">
+      <c r="I2" s="154" t="s">
         <v>215</v>
       </c>
-      <c r="J2" s="161"/>
-      <c r="K2" s="161"/>
-      <c r="L2" s="161"/>
-      <c r="M2" s="161"/>
-      <c r="N2" s="161"/>
-      <c r="O2" s="161"/>
-      <c r="P2" s="161"/>
-      <c r="Q2" s="161"/>
-      <c r="R2" s="161"/>
-      <c r="S2" s="161"/>
-      <c r="T2" s="161"/>
-      <c r="U2" s="161"/>
-      <c r="V2" s="161"/>
-      <c r="W2" s="161"/>
-      <c r="X2" s="161"/>
-      <c r="Y2" s="161"/>
-      <c r="Z2" s="161"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
+      <c r="P2" s="154"/>
+      <c r="Q2" s="154"/>
+      <c r="R2" s="154"/>
+      <c r="S2" s="154"/>
+      <c r="T2" s="154"/>
+      <c r="U2" s="154"/>
+      <c r="V2" s="154"/>
+      <c r="W2" s="154"/>
+      <c r="X2" s="154"/>
+      <c r="Y2" s="154"/>
+      <c r="Z2" s="154"/>
     </row>
     <row r="5" spans="2:34">
-      <c r="D5" s="153" t="s">
+      <c r="D5" s="159" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="151" t="s">
+      <c r="E5" s="150" t="s">
         <v>217</v>
       </c>
-      <c r="F5" s="157" t="s">
+      <c r="F5" s="152" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="158"/>
-      <c r="H5" s="157" t="s">
+      <c r="G5" s="153"/>
+      <c r="H5" s="152" t="s">
         <v>229</v>
       </c>
-      <c r="I5" s="159"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
-      <c r="O5" s="158"/>
-      <c r="P5" s="157" t="s">
+      <c r="I5" s="163"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="163"/>
+      <c r="L5" s="163"/>
+      <c r="M5" s="163"/>
+      <c r="N5" s="163"/>
+      <c r="O5" s="153"/>
+      <c r="P5" s="152" t="s">
         <v>228</v>
       </c>
-      <c r="Q5" s="159"/>
-      <c r="R5" s="159"/>
-      <c r="S5" s="159"/>
-      <c r="T5" s="159"/>
-      <c r="U5" s="159"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="157" t="s">
+      <c r="Q5" s="163"/>
+      <c r="R5" s="163"/>
+      <c r="S5" s="163"/>
+      <c r="T5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="153"/>
+      <c r="W5" s="152" t="s">
         <v>135</v>
       </c>
-      <c r="X5" s="158"/>
-      <c r="Y5" s="162" t="s">
+      <c r="X5" s="153"/>
+      <c r="Y5" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="Z5" s="162"/>
+      <c r="Z5" s="157"/>
       <c r="AA5" s="75"/>
       <c r="AB5" s="75"/>
     </row>
     <row r="6" spans="2:34" ht="15" customHeight="1">
-      <c r="D6" s="154"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="151" t="s">
+      <c r="D6" s="160"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="150" t="s">
         <v>218</v>
       </c>
-      <c r="G6" s="151" t="s">
+      <c r="G6" s="150" t="s">
         <v>219</v>
       </c>
-      <c r="H6" s="151" t="s">
+      <c r="H6" s="150" t="s">
         <v>220</v>
       </c>
-      <c r="I6" s="151" t="s">
+      <c r="I6" s="150" t="s">
         <v>221</v>
       </c>
-      <c r="J6" s="151" t="s">
+      <c r="J6" s="150" t="s">
         <v>222</v>
       </c>
-      <c r="K6" s="149" t="s">
+      <c r="K6" s="155" t="s">
         <v>223</v>
       </c>
-      <c r="L6" s="151" t="s">
+      <c r="L6" s="150" t="s">
         <v>230</v>
       </c>
-      <c r="M6" s="151" t="s">
+      <c r="M6" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="160" t="s">
+      <c r="N6" s="158" t="s">
         <v>135</v>
       </c>
-      <c r="O6" s="160"/>
-      <c r="P6" s="149" t="s">
+      <c r="O6" s="158"/>
+      <c r="P6" s="155" t="s">
         <v>224</v>
       </c>
-      <c r="Q6" s="151" t="s">
+      <c r="Q6" s="150" t="s">
         <v>225</v>
       </c>
-      <c r="R6" s="151" t="s">
+      <c r="R6" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="S6" s="149" t="s">
+      <c r="S6" s="155" t="s">
         <v>226</v>
       </c>
-      <c r="T6" s="149" t="s">
+      <c r="T6" s="155" t="s">
         <v>231</v>
       </c>
-      <c r="U6" s="149" t="s">
+      <c r="U6" s="155" t="s">
         <v>12</v>
       </c>
-      <c r="V6" s="151" t="s">
+      <c r="V6" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="W6" s="151" t="s">
+      <c r="W6" s="150" t="s">
         <v>227</v>
       </c>
-      <c r="X6" s="151" t="s">
+      <c r="X6" s="150" t="s">
         <v>219</v>
       </c>
-      <c r="Y6" s="160" t="s">
+      <c r="Y6" s="158" t="s">
         <v>218</v>
       </c>
-      <c r="Z6" s="160" t="s">
+      <c r="Z6" s="158" t="s">
         <v>219</v>
       </c>
       <c r="AA6" s="76"/>
       <c r="AB6" s="76"/>
     </row>
     <row r="7" spans="2:34">
-      <c r="D7" s="155"/>
-      <c r="E7" s="152"/>
-      <c r="F7" s="152"/>
-      <c r="G7" s="152"/>
-      <c r="H7" s="152"/>
-      <c r="I7" s="152"/>
-      <c r="J7" s="152"/>
-      <c r="K7" s="150"/>
-      <c r="L7" s="152"/>
-      <c r="M7" s="152"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="151"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="151"/>
+      <c r="H7" s="151"/>
+      <c r="I7" s="151"/>
+      <c r="J7" s="151"/>
+      <c r="K7" s="156"/>
+      <c r="L7" s="151"/>
+      <c r="M7" s="151"/>
       <c r="N7" s="77" t="s">
         <v>218</v>
       </c>
       <c r="O7" s="71" t="s">
         <v>219</v>
       </c>
-      <c r="P7" s="150"/>
-      <c r="Q7" s="152"/>
-      <c r="R7" s="152"/>
-      <c r="S7" s="150"/>
-      <c r="T7" s="150"/>
-      <c r="U7" s="150"/>
-      <c r="V7" s="152"/>
-      <c r="W7" s="152"/>
-      <c r="X7" s="152"/>
-      <c r="Y7" s="160"/>
-      <c r="Z7" s="160"/>
+      <c r="P7" s="156"/>
+      <c r="Q7" s="151"/>
+      <c r="R7" s="151"/>
+      <c r="S7" s="156"/>
+      <c r="T7" s="156"/>
+      <c r="U7" s="156"/>
+      <c r="V7" s="151"/>
+      <c r="W7" s="151"/>
+      <c r="X7" s="151"/>
+      <c r="Y7" s="158"/>
+      <c r="Z7" s="158"/>
       <c r="AA7" s="76"/>
       <c r="AB7" s="76"/>
     </row>
@@ -38388,6 +38391,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P5:V5"/>
+    <mergeCell ref="V6:V7"/>
     <mergeCell ref="X6:X7"/>
     <mergeCell ref="W5:X5"/>
     <mergeCell ref="I2:Z2"/>
@@ -38404,18 +38419,6 @@
     <mergeCell ref="Y6:Y7"/>
     <mergeCell ref="Z6:Z7"/>
     <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H5:O5"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P5:V5"/>
-    <mergeCell ref="V6:V7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -38457,28 +38460,28 @@
     <row r="2" spans="2:29" ht="33" customHeight="1">
       <c r="B2" s="11"/>
       <c r="C2" s="20"/>
-      <c r="D2" s="166" t="s">
+      <c r="D2" s="164" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="166"/>
-      <c r="I2" s="166" t="s">
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="166"/>
-      <c r="K2" s="166"/>
-      <c r="L2" s="166"/>
-      <c r="M2" s="166"/>
-      <c r="N2" s="166"/>
-      <c r="O2" s="166"/>
-      <c r="R2" s="167" t="s">
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
+      <c r="L2" s="164"/>
+      <c r="M2" s="164"/>
+      <c r="N2" s="164"/>
+      <c r="O2" s="164"/>
+      <c r="R2" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="170"/>
-      <c r="T2" s="170"/>
-      <c r="U2" s="168"/>
+      <c r="S2" s="166"/>
+      <c r="T2" s="166"/>
+      <c r="U2" s="167"/>
     </row>
     <row r="4" spans="2:29" ht="15" customHeight="1">
       <c r="C4" s="21" t="s">
@@ -45742,32 +45745,32 @@
     </row>
     <row r="2" spans="1:27" ht="33" customHeight="1">
       <c r="A2" s="41"/>
-      <c r="B2" s="172" t="s">
+      <c r="B2" s="170" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
       <c r="G2" s="59"/>
-      <c r="H2" s="172" t="s">
+      <c r="H2" s="170" t="s">
         <v>166</v>
       </c>
-      <c r="I2" s="172"/>
-      <c r="J2" s="172"/>
-      <c r="K2" s="172"/>
-      <c r="L2" s="172"/>
-      <c r="M2" s="172"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
+      <c r="L2" s="170"/>
+      <c r="M2" s="170"/>
       <c r="N2" s="59"/>
       <c r="O2" s="59"/>
       <c r="P2" s="59"/>
       <c r="Q2" s="59"/>
       <c r="R2" s="89"/>
       <c r="S2" s="89"/>
-      <c r="T2" s="174" t="s">
+      <c r="T2" s="176" t="s">
         <v>167</v>
       </c>
-      <c r="U2" s="175"/>
+      <c r="U2" s="177"/>
       <c r="V2" s="41"/>
       <c r="W2" s="41"/>
       <c r="X2" s="41"/>
@@ -45832,38 +45835,38 @@
       <c r="B5" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="176" t="s">
+      <c r="C5" s="172" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="176" t="s">
+      <c r="D5" s="172" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="176"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="176"/>
-      <c r="H5" s="176" t="s">
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="172"/>
+      <c r="H5" s="172" t="s">
         <v>107</v>
       </c>
-      <c r="I5" s="176"/>
-      <c r="J5" s="176"/>
-      <c r="K5" s="176"/>
-      <c r="L5" s="176"/>
-      <c r="M5" s="176" t="s">
+      <c r="I5" s="172"/>
+      <c r="J5" s="172"/>
+      <c r="K5" s="172"/>
+      <c r="L5" s="172"/>
+      <c r="M5" s="172" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="176"/>
-      <c r="O5" s="176"/>
-      <c r="P5" s="176"/>
-      <c r="Q5" s="176"/>
-      <c r="R5" s="176"/>
-      <c r="S5" s="176"/>
-      <c r="T5" s="176" t="s">
+      <c r="N5" s="172"/>
+      <c r="O5" s="172"/>
+      <c r="P5" s="172"/>
+      <c r="Q5" s="172"/>
+      <c r="R5" s="172"/>
+      <c r="S5" s="172"/>
+      <c r="T5" s="172" t="s">
         <v>119</v>
       </c>
-      <c r="U5" s="176" t="s">
+      <c r="U5" s="172" t="s">
         <v>120</v>
       </c>
-      <c r="V5" s="177"/>
+      <c r="V5" s="178"/>
       <c r="W5" s="41"/>
       <c r="X5" s="41"/>
       <c r="Y5" s="41"/>
@@ -45871,48 +45874,48 @@
     <row r="6" spans="1:27">
       <c r="A6" s="41"/>
       <c r="B6" s="180"/>
-      <c r="C6" s="178"/>
-      <c r="D6" s="178" t="s">
+      <c r="C6" s="173"/>
+      <c r="D6" s="173" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="178" t="s">
+      <c r="E6" s="173" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="178" t="s">
+      <c r="F6" s="173" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="178" t="s">
+      <c r="G6" s="173" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="178" t="s">
+      <c r="H6" s="173" t="s">
         <v>110</v>
       </c>
-      <c r="I6" s="178"/>
-      <c r="J6" s="178" t="s">
+      <c r="I6" s="173"/>
+      <c r="J6" s="173" t="s">
         <v>111</v>
       </c>
-      <c r="K6" s="178"/>
+      <c r="K6" s="173"/>
       <c r="L6" s="84" t="s">
         <v>112</v>
       </c>
-      <c r="M6" s="178" t="s">
+      <c r="M6" s="173" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="178"/>
-      <c r="O6" s="178"/>
-      <c r="P6" s="178" t="s">
+      <c r="N6" s="173"/>
+      <c r="O6" s="173"/>
+      <c r="P6" s="173" t="s">
         <v>117</v>
       </c>
-      <c r="Q6" s="178"/>
-      <c r="R6" s="178"/>
-      <c r="S6" s="178" t="s">
+      <c r="Q6" s="173"/>
+      <c r="R6" s="173"/>
+      <c r="S6" s="173" t="s">
         <v>112</v>
       </c>
-      <c r="T6" s="178"/>
-      <c r="U6" s="178" t="s">
+      <c r="T6" s="173"/>
+      <c r="U6" s="173" t="s">
         <v>121</v>
       </c>
-      <c r="V6" s="171" t="s">
+      <c r="V6" s="174" t="s">
         <v>122</v>
       </c>
       <c r="W6" s="41"/>
@@ -45922,11 +45925,11 @@
     <row r="7" spans="1:27">
       <c r="A7" s="41"/>
       <c r="B7" s="180"/>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="178"/>
+      <c r="C7" s="173"/>
+      <c r="D7" s="173"/>
+      <c r="E7" s="173"/>
+      <c r="F7" s="173"/>
+      <c r="G7" s="173"/>
       <c r="H7" s="84" t="s">
         <v>108</v>
       </c>
@@ -45960,10 +45963,10 @@
       <c r="R7" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="178"/>
-      <c r="T7" s="178"/>
-      <c r="U7" s="178"/>
-      <c r="V7" s="171"/>
+      <c r="S7" s="173"/>
+      <c r="T7" s="173"/>
+      <c r="U7" s="173"/>
+      <c r="V7" s="174"/>
       <c r="W7" s="41"/>
       <c r="X7" s="41"/>
       <c r="Y7" s="41"/>
@@ -53472,11 +53475,11 @@
       <c r="P103" s="41"/>
       <c r="Q103" s="41"/>
       <c r="R103" s="41"/>
-      <c r="S103" s="181" t="s">
+      <c r="S103" s="168" t="s">
         <v>318</v>
       </c>
-      <c r="T103" s="181"/>
-      <c r="U103" s="181"/>
+      <c r="T103" s="168"/>
+      <c r="U103" s="168"/>
       <c r="V103" s="41"/>
       <c r="W103" s="41"/>
       <c r="X103" s="41"/>
@@ -53485,31 +53488,31 @@
     <row r="104" spans="1:27" s="5" customFormat="1" ht="63" customHeight="1">
       <c r="A104" s="91"/>
       <c r="B104" s="85"/>
-      <c r="C104" s="182" t="s">
+      <c r="C104" s="169" t="s">
         <v>308</v>
       </c>
-      <c r="D104" s="182"/>
+      <c r="D104" s="169"/>
       <c r="E104" s="91"/>
       <c r="F104" s="91"/>
       <c r="G104" s="91"/>
       <c r="H104" s="91"/>
       <c r="I104" s="91"/>
       <c r="J104" s="91"/>
-      <c r="K104" s="182" t="s">
+      <c r="K104" s="169" t="s">
         <v>309</v>
       </c>
-      <c r="L104" s="182"/>
-      <c r="M104" s="182"/>
+      <c r="L104" s="169"/>
+      <c r="M104" s="169"/>
       <c r="N104" s="91"/>
       <c r="O104" s="91"/>
       <c r="P104" s="91"/>
       <c r="Q104" s="91"/>
       <c r="R104" s="91"/>
-      <c r="S104" s="183" t="s">
+      <c r="S104" s="171" t="s">
         <v>339</v>
       </c>
-      <c r="T104" s="183"/>
-      <c r="U104" s="183"/>
+      <c r="T104" s="171"/>
+      <c r="U104" s="171"/>
       <c r="V104" s="91"/>
       <c r="W104" s="91"/>
       <c r="X104" s="91"/>
@@ -53601,31 +53604,31 @@
     <row r="108" spans="1:27" s="5" customFormat="1">
       <c r="A108" s="91"/>
       <c r="B108" s="85"/>
-      <c r="C108" s="182" t="s">
+      <c r="C108" s="169" t="s">
         <v>312</v>
       </c>
-      <c r="D108" s="182"/>
+      <c r="D108" s="169"/>
       <c r="E108" s="91"/>
       <c r="F108" s="91"/>
       <c r="G108" s="91"/>
       <c r="H108" s="91"/>
       <c r="I108" s="91"/>
       <c r="J108" s="91"/>
-      <c r="K108" s="182" t="s">
+      <c r="K108" s="169" t="s">
         <v>313</v>
       </c>
-      <c r="L108" s="182"/>
-      <c r="M108" s="182"/>
+      <c r="L108" s="169"/>
+      <c r="M108" s="169"/>
       <c r="N108" s="91"/>
       <c r="O108" s="91"/>
       <c r="P108" s="91"/>
       <c r="Q108" s="91"/>
       <c r="R108" s="91"/>
-      <c r="S108" s="182" t="s">
+      <c r="S108" s="169" t="s">
         <v>314</v>
       </c>
-      <c r="T108" s="182"/>
-      <c r="U108" s="182"/>
+      <c r="T108" s="169"/>
+      <c r="U108" s="169"/>
       <c r="V108" s="91"/>
       <c r="W108" s="91"/>
       <c r="X108" s="91"/>
@@ -53986,6 +53989,20 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="B5:B7"/>
     <mergeCell ref="S103:U103"/>
     <mergeCell ref="S108:U108"/>
     <mergeCell ref="H2:M2"/>
@@ -54000,20 +54017,6 @@
     <mergeCell ref="M5:S5"/>
     <mergeCell ref="T5:T7"/>
     <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" orientation="landscape" r:id="rId1"/>
@@ -54048,117 +54051,117 @@
         <v>125</v>
       </c>
       <c r="S2" s="35"/>
-      <c r="AA2" s="185" t="s">
+      <c r="AA2" s="182" t="s">
         <v>143</v>
       </c>
-      <c r="AB2" s="186"/>
+      <c r="AB2" s="183"/>
     </row>
     <row r="5" spans="2:30">
-      <c r="B5" s="184" t="s">
+      <c r="B5" s="181" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
-      <c r="E5" s="184" t="s">
+      <c r="E5" s="181" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="184" t="s">
+      <c r="F5" s="181" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="184"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
-      <c r="J5" s="184" t="s">
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181" t="s">
         <v>131</v>
       </c>
-      <c r="K5" s="184"/>
-      <c r="L5" s="184"/>
-      <c r="M5" s="184" t="s">
+      <c r="K5" s="181"/>
+      <c r="L5" s="181"/>
+      <c r="M5" s="181" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="184"/>
-      <c r="O5" s="184"/>
-      <c r="P5" s="184" t="s">
+      <c r="N5" s="181"/>
+      <c r="O5" s="181"/>
+      <c r="P5" s="181" t="s">
         <v>134</v>
       </c>
-      <c r="Q5" s="184" t="s">
+      <c r="Q5" s="181" t="s">
         <v>135</v>
       </c>
-      <c r="R5" s="184" t="s">
+      <c r="R5" s="181" t="s">
         <v>136</v>
       </c>
-      <c r="S5" s="184"/>
-      <c r="T5" s="184"/>
-      <c r="U5" s="184"/>
-      <c r="V5" s="184" t="s">
+      <c r="S5" s="181"/>
+      <c r="T5" s="181"/>
+      <c r="U5" s="181"/>
+      <c r="V5" s="181" t="s">
         <v>138</v>
       </c>
-      <c r="W5" s="184"/>
-      <c r="X5" s="184" t="s">
+      <c r="W5" s="181"/>
+      <c r="X5" s="181" t="s">
         <v>139</v>
       </c>
-      <c r="Y5" s="184"/>
-      <c r="Z5" s="184" t="s">
+      <c r="Y5" s="181"/>
+      <c r="Z5" s="181" t="s">
         <v>140</v>
       </c>
-      <c r="AA5" s="184"/>
-      <c r="AB5" s="184"/>
-      <c r="AC5" s="184"/>
-      <c r="AD5" s="184" t="s">
+      <c r="AA5" s="181"/>
+      <c r="AB5" s="181"/>
+      <c r="AC5" s="181"/>
+      <c r="AD5" s="181" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:30">
-      <c r="B6" s="184"/>
+      <c r="B6" s="181"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
-      <c r="E6" s="184"/>
-      <c r="F6" s="184" t="s">
+      <c r="E6" s="181"/>
+      <c r="F6" s="181" t="s">
         <v>128</v>
       </c>
-      <c r="G6" s="184"/>
-      <c r="H6" s="184"/>
-      <c r="I6" s="184" t="s">
+      <c r="G6" s="181"/>
+      <c r="H6" s="181"/>
+      <c r="I6" s="181" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="184" t="s">
+      <c r="J6" s="181" t="s">
         <v>212</v>
       </c>
-      <c r="K6" s="184" t="s">
+      <c r="K6" s="181" t="s">
         <v>129</v>
       </c>
-      <c r="L6" s="184" t="s">
+      <c r="L6" s="181" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="184" t="s">
+      <c r="M6" s="181" t="s">
         <v>132</v>
       </c>
-      <c r="N6" s="184" t="s">
+      <c r="N6" s="181" t="s">
         <v>133</v>
       </c>
-      <c r="O6" s="184" t="s">
+      <c r="O6" s="181" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="184"/>
-      <c r="Q6" s="184"/>
-      <c r="R6" s="184" t="s">
+      <c r="P6" s="181"/>
+      <c r="Q6" s="181"/>
+      <c r="R6" s="181" t="s">
         <v>128</v>
       </c>
-      <c r="S6" s="184"/>
-      <c r="T6" s="184" t="s">
+      <c r="S6" s="181"/>
+      <c r="T6" s="181" t="s">
         <v>137</v>
       </c>
-      <c r="U6" s="184"/>
-      <c r="V6" s="184" t="s">
+      <c r="U6" s="181"/>
+      <c r="V6" s="181" t="s">
         <v>129</v>
       </c>
-      <c r="W6" s="184" t="s">
+      <c r="W6" s="181" t="s">
         <v>130</v>
       </c>
-      <c r="X6" s="184" t="s">
+      <c r="X6" s="181" t="s">
         <v>129</v>
       </c>
-      <c r="Y6" s="184" t="s">
+      <c r="Y6" s="181" t="s">
         <v>130</v>
       </c>
       <c r="Z6" s="33" t="s">
@@ -54169,13 +54172,13 @@
         <v>133</v>
       </c>
       <c r="AC6" s="33"/>
-      <c r="AD6" s="184"/>
+      <c r="AD6" s="181"/>
     </row>
     <row r="7" spans="2:30">
-      <c r="B7" s="184"/>
+      <c r="B7" s="181"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
-      <c r="E7" s="184"/>
+      <c r="E7" s="181"/>
       <c r="F7" s="33" t="s">
         <v>212</v>
       </c>
@@ -54185,15 +54188,15 @@
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="184"/>
-      <c r="J7" s="184"/>
-      <c r="K7" s="184"/>
-      <c r="L7" s="184"/>
-      <c r="M7" s="184"/>
-      <c r="N7" s="184"/>
-      <c r="O7" s="184"/>
-      <c r="P7" s="184"/>
-      <c r="Q7" s="184"/>
+      <c r="I7" s="181"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="181"/>
+      <c r="M7" s="181"/>
+      <c r="N7" s="181"/>
+      <c r="O7" s="181"/>
+      <c r="P7" s="181"/>
+      <c r="Q7" s="181"/>
       <c r="R7" s="33" t="s">
         <v>121</v>
       </c>
@@ -54206,10 +54209,10 @@
       <c r="U7" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="V7" s="184"/>
-      <c r="W7" s="184"/>
-      <c r="X7" s="184"/>
-      <c r="Y7" s="184"/>
+      <c r="V7" s="181"/>
+      <c r="W7" s="181"/>
+      <c r="X7" s="181"/>
+      <c r="Y7" s="181"/>
       <c r="Z7" s="33" t="s">
         <v>122</v>
       </c>
@@ -54222,7 +54225,7 @@
       <c r="AC7" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="AD7" s="184"/>
+      <c r="AD7" s="181"/>
     </row>
     <row r="9" spans="2:30" s="5" customFormat="1">
       <c r="B9" s="5" t="s">
@@ -66649,6 +66652,24 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="Q5:Q7"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
     <mergeCell ref="AD5:AD7"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="W6:W7"/>
@@ -66658,24 +66679,6 @@
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="Z5:AC5"/>
     <mergeCell ref="V6:V7"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="Q5:Q7"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="I6:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -66701,34 +66704,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:28" s="44" customFormat="1" ht="35.25" customHeight="1">
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="193" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="198" t="s">
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="192" t="s">
         <v>164</v>
       </c>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
-      <c r="P2" s="198"/>
-      <c r="Q2" s="198"/>
-      <c r="R2" s="198"/>
-      <c r="S2" s="198"/>
+      <c r="J2" s="192"/>
+      <c r="K2" s="192"/>
+      <c r="L2" s="192"/>
+      <c r="M2" s="192"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="192"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="192"/>
+      <c r="R2" s="192"/>
+      <c r="S2" s="192"/>
       <c r="T2" s="43"/>
       <c r="U2" s="43"/>
-      <c r="Y2" s="192" t="s">
+      <c r="Y2" s="184" t="s">
         <v>143</v>
       </c>
-      <c r="Z2" s="193"/>
+      <c r="Z2" s="185"/>
     </row>
     <row r="3" spans="2:28">
       <c r="Q3" s="37"/>
@@ -66763,76 +66766,76 @@
       <c r="AB4" s="7"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" thickTop="1">
-      <c r="B5" s="194" t="s">
+      <c r="B5" s="186" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="196" t="s">
+      <c r="C5" s="188" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="196" t="s">
+      <c r="D5" s="188" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="196"/>
-      <c r="F5" s="196"/>
-      <c r="G5" s="196"/>
-      <c r="H5" s="196" t="s">
+      <c r="E5" s="188"/>
+      <c r="F5" s="188"/>
+      <c r="G5" s="188"/>
+      <c r="H5" s="188" t="s">
         <v>131</v>
       </c>
-      <c r="I5" s="196"/>
-      <c r="J5" s="196"/>
-      <c r="K5" s="196" t="s">
+      <c r="I5" s="188"/>
+      <c r="J5" s="188"/>
+      <c r="K5" s="188" t="s">
         <v>113</v>
       </c>
-      <c r="L5" s="196"/>
-      <c r="M5" s="196"/>
-      <c r="N5" s="197" t="s">
+      <c r="L5" s="188"/>
+      <c r="M5" s="188"/>
+      <c r="N5" s="190" t="s">
         <v>134</v>
       </c>
-      <c r="O5" s="197" t="s">
+      <c r="O5" s="190" t="s">
         <v>135</v>
       </c>
-      <c r="P5" s="196" t="s">
+      <c r="P5" s="188" t="s">
         <v>136</v>
       </c>
-      <c r="Q5" s="196"/>
-      <c r="R5" s="196"/>
-      <c r="S5" s="196"/>
-      <c r="T5" s="197" t="s">
+      <c r="Q5" s="188"/>
+      <c r="R5" s="188"/>
+      <c r="S5" s="188"/>
+      <c r="T5" s="190" t="s">
         <v>138</v>
       </c>
-      <c r="U5" s="197"/>
-      <c r="V5" s="196" t="s">
+      <c r="U5" s="190"/>
+      <c r="V5" s="188" t="s">
         <v>139</v>
       </c>
-      <c r="W5" s="196"/>
-      <c r="X5" s="196" t="s">
+      <c r="W5" s="188"/>
+      <c r="X5" s="188" t="s">
         <v>140</v>
       </c>
-      <c r="Y5" s="196"/>
-      <c r="Z5" s="196"/>
-      <c r="AA5" s="196"/>
-      <c r="AB5" s="188" t="s">
+      <c r="Y5" s="188"/>
+      <c r="Z5" s="188"/>
+      <c r="AA5" s="188"/>
+      <c r="AB5" s="195" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:28">
-      <c r="B6" s="195"/>
-      <c r="C6" s="190"/>
-      <c r="D6" s="190" t="s">
+      <c r="B6" s="187"/>
+      <c r="C6" s="189"/>
+      <c r="D6" s="189" t="s">
         <v>128</v>
       </c>
-      <c r="E6" s="190"/>
-      <c r="F6" s="190"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="189"/>
       <c r="G6" s="191" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="190" t="s">
+      <c r="H6" s="189" t="s">
         <v>133</v>
       </c>
-      <c r="I6" s="190" t="s">
+      <c r="I6" s="189" t="s">
         <v>132</v>
       </c>
-      <c r="J6" s="190" t="s">
+      <c r="J6" s="189" t="s">
         <v>7</v>
       </c>
       <c r="K6" s="191" t="s">
@@ -66846,24 +66849,24 @@
       </c>
       <c r="N6" s="191"/>
       <c r="O6" s="191"/>
-      <c r="P6" s="190" t="s">
+      <c r="P6" s="189" t="s">
         <v>128</v>
       </c>
-      <c r="Q6" s="190"/>
-      <c r="R6" s="190" t="s">
+      <c r="Q6" s="189"/>
+      <c r="R6" s="189" t="s">
         <v>137</v>
       </c>
-      <c r="S6" s="190"/>
+      <c r="S6" s="189"/>
       <c r="T6" s="191" t="s">
         <v>129</v>
       </c>
       <c r="U6" s="191" t="s">
         <v>130</v>
       </c>
-      <c r="V6" s="190" t="s">
+      <c r="V6" s="189" t="s">
         <v>129</v>
       </c>
-      <c r="W6" s="190" t="s">
+      <c r="W6" s="189" t="s">
         <v>130</v>
       </c>
       <c r="X6" s="2" t="s">
@@ -66874,11 +66877,11 @@
         <v>133</v>
       </c>
       <c r="AA6" s="2"/>
-      <c r="AB6" s="189"/>
+      <c r="AB6" s="196"/>
     </row>
     <row r="7" spans="2:28">
-      <c r="B7" s="195"/>
-      <c r="C7" s="190"/>
+      <c r="B7" s="187"/>
+      <c r="C7" s="189"/>
       <c r="D7" s="2" t="s">
         <v>129</v>
       </c>
@@ -66889,9 +66892,9 @@
         <v>7</v>
       </c>
       <c r="G7" s="191"/>
-      <c r="H7" s="190"/>
-      <c r="I7" s="190"/>
-      <c r="J7" s="190"/>
+      <c r="H7" s="189"/>
+      <c r="I7" s="189"/>
+      <c r="J7" s="189"/>
       <c r="K7" s="191"/>
       <c r="L7" s="191"/>
       <c r="M7" s="191"/>
@@ -66911,8 +66914,8 @@
       </c>
       <c r="T7" s="191"/>
       <c r="U7" s="191"/>
-      <c r="V7" s="190"/>
-      <c r="W7" s="190"/>
+      <c r="V7" s="189"/>
+      <c r="W7" s="189"/>
       <c r="X7" s="2" t="s">
         <v>122</v>
       </c>
@@ -66925,7 +66928,7 @@
       <c r="AA7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AB7" s="189"/>
+      <c r="AB7" s="196"/>
     </row>
     <row r="8" spans="2:28" s="5" customFormat="1">
       <c r="B8" s="27" t="str">
@@ -80468,68 +80471,91 @@
       <c r="C193" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="F193" s="161" t="s">
+      <c r="F193" s="154" t="s">
         <v>463</v>
       </c>
-      <c r="G193" s="161"/>
-      <c r="J193" s="161" t="s">
+      <c r="G193" s="154"/>
+      <c r="J193" s="154" t="s">
         <v>465</v>
       </c>
-      <c r="K193" s="161"/>
-      <c r="L193" s="161"/>
+      <c r="K193" s="154"/>
+      <c r="L193" s="154"/>
       <c r="M193" s="115"/>
       <c r="N193" s="115"/>
-      <c r="O193" s="187" t="s">
+      <c r="O193" s="194" t="s">
         <v>467</v>
       </c>
-      <c r="P193" s="187"/>
-      <c r="Q193" s="187"/>
-      <c r="T193" s="187" t="s">
+      <c r="P193" s="194"/>
+      <c r="Q193" s="194"/>
+      <c r="T193" s="194" t="s">
         <v>469</v>
       </c>
-      <c r="U193" s="187"/>
-      <c r="V193" s="187"/>
-      <c r="Y193" s="161" t="s">
+      <c r="U193" s="194"/>
+      <c r="V193" s="194"/>
+      <c r="Y193" s="154" t="s">
         <v>471</v>
       </c>
-      <c r="Z193" s="161"/>
-      <c r="AA193" s="161"/>
+      <c r="Z193" s="154"/>
+      <c r="AA193" s="154"/>
     </row>
     <row r="197" spans="2:27" s="5" customFormat="1">
       <c r="B197" s="114"/>
       <c r="C197" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="F197" s="161" t="s">
+      <c r="F197" s="154" t="s">
         <v>464</v>
       </c>
-      <c r="G197" s="161"/>
+      <c r="G197" s="154"/>
       <c r="H197" s="66"/>
-      <c r="J197" s="161" t="s">
+      <c r="J197" s="154" t="s">
         <v>466</v>
       </c>
-      <c r="K197" s="161"/>
-      <c r="L197" s="161"/>
+      <c r="K197" s="154"/>
+      <c r="L197" s="154"/>
       <c r="M197" s="115"/>
       <c r="N197" s="115"/>
-      <c r="O197" s="187" t="s">
+      <c r="O197" s="194" t="s">
         <v>468</v>
       </c>
-      <c r="P197" s="187"/>
-      <c r="Q197" s="187"/>
-      <c r="T197" s="187" t="s">
+      <c r="P197" s="194"/>
+      <c r="Q197" s="194"/>
+      <c r="T197" s="194" t="s">
         <v>470</v>
       </c>
-      <c r="U197" s="187"/>
-      <c r="V197" s="187"/>
-      <c r="Y197" s="161" t="s">
+      <c r="U197" s="194"/>
+      <c r="V197" s="194"/>
+      <c r="Y197" s="154" t="s">
         <v>472</v>
       </c>
-      <c r="Z197" s="161"/>
-      <c r="AA197" s="161"/>
+      <c r="Z197" s="154"/>
+      <c r="AA197" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="T197:V197"/>
+    <mergeCell ref="T193:V193"/>
+    <mergeCell ref="Y197:AA197"/>
+    <mergeCell ref="Y193:AA193"/>
+    <mergeCell ref="AB5:AB7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="F193:G193"/>
+    <mergeCell ref="F197:G197"/>
+    <mergeCell ref="J197:L197"/>
+    <mergeCell ref="J193:L193"/>
+    <mergeCell ref="O193:Q193"/>
+    <mergeCell ref="O197:Q197"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
@@ -80546,29 +80572,6 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
-    <mergeCell ref="F193:G193"/>
-    <mergeCell ref="F197:G197"/>
-    <mergeCell ref="J197:L197"/>
-    <mergeCell ref="J193:L193"/>
-    <mergeCell ref="O193:Q193"/>
-    <mergeCell ref="O197:Q197"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="T197:V197"/>
-    <mergeCell ref="T193:V193"/>
-    <mergeCell ref="Y197:AA197"/>
-    <mergeCell ref="Y193:AA193"/>
-    <mergeCell ref="AB5:AB7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="V6:V7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -80581,7 +80584,7 @@
   <dimension ref="A1:AG21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -80633,24 +80636,24 @@
     </row>
     <row r="2" spans="1:32" ht="42.75" customHeight="1">
       <c r="G2" s="21"/>
-      <c r="H2" s="166" t="s">
+      <c r="H2" s="164" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="166"/>
-      <c r="J2" s="166"/>
-      <c r="K2" s="166"/>
-      <c r="L2" s="166"/>
-      <c r="M2" s="169" t="s">
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
+      <c r="L2" s="164"/>
+      <c r="M2" s="197" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="169"/>
-      <c r="O2" s="169"/>
-      <c r="P2" s="169"/>
-      <c r="Q2" s="169"/>
-      <c r="R2" s="169"/>
-      <c r="S2" s="169"/>
-      <c r="T2" s="169"/>
-      <c r="U2" s="169"/>
+      <c r="N2" s="197"/>
+      <c r="O2" s="197"/>
+      <c r="P2" s="197"/>
+      <c r="Q2" s="197"/>
+      <c r="R2" s="197"/>
+      <c r="S2" s="197"/>
+      <c r="T2" s="197"/>
+      <c r="U2" s="197"/>
       <c r="V2" s="105"/>
       <c r="W2" s="105"/>
       <c r="X2" s="105"/>
@@ -80659,10 +80662,10 @@
       <c r="AA2" s="106"/>
       <c r="AB2" s="106"/>
       <c r="AC2" s="106"/>
-      <c r="AD2" s="167" t="s">
+      <c r="AD2" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="AE2" s="168"/>
+      <c r="AE2" s="167"/>
       <c r="AF2" s="106"/>
     </row>
     <row r="3" spans="1:32" hidden="1">
@@ -80807,7 +80810,7 @@
     </row>
     <row r="8" spans="1:32" s="142" customFormat="1">
       <c r="G8" s="143"/>
-      <c r="H8" s="143"/>
+      <c r="H8" s="147"/>
       <c r="I8" s="144"/>
       <c r="J8" s="144"/>
       <c r="K8" s="144"/>
@@ -80834,60 +80837,60 @@
       <c r="AF8" s="144"/>
     </row>
     <row r="9" spans="1:32" s="145" customFormat="1">
-      <c r="G9" s="227"/>
-      <c r="H9" s="227"/>
-      <c r="I9" s="227"/>
-      <c r="J9" s="227"/>
-      <c r="K9" s="227"/>
-      <c r="L9" s="227"/>
-      <c r="M9" s="227"/>
-      <c r="N9" s="227"/>
-      <c r="O9" s="227"/>
-      <c r="P9" s="227"/>
-      <c r="Q9" s="227"/>
-      <c r="R9" s="227"/>
-      <c r="S9" s="227"/>
-      <c r="T9" s="227"/>
-      <c r="U9" s="227"/>
-      <c r="V9" s="227"/>
-      <c r="W9" s="227"/>
-      <c r="X9" s="227"/>
-      <c r="Y9" s="227"/>
-      <c r="Z9" s="227"/>
-      <c r="AA9" s="227"/>
-      <c r="AB9" s="227"/>
-      <c r="AC9" s="227"/>
-      <c r="AD9" s="227"/>
-      <c r="AE9" s="227"/>
-      <c r="AF9" s="227"/>
+      <c r="G9" s="149"/>
+      <c r="H9" s="228"/>
+      <c r="I9" s="149"/>
+      <c r="J9" s="149"/>
+      <c r="K9" s="149"/>
+      <c r="L9" s="149"/>
+      <c r="M9" s="149"/>
+      <c r="N9" s="149"/>
+      <c r="O9" s="149"/>
+      <c r="P9" s="149"/>
+      <c r="Q9" s="149"/>
+      <c r="R9" s="149"/>
+      <c r="S9" s="149"/>
+      <c r="T9" s="149"/>
+      <c r="U9" s="149"/>
+      <c r="V9" s="149"/>
+      <c r="W9" s="149"/>
+      <c r="X9" s="149"/>
+      <c r="Y9" s="149"/>
+      <c r="Z9" s="149"/>
+      <c r="AA9" s="149"/>
+      <c r="AB9" s="149"/>
+      <c r="AC9" s="149"/>
+      <c r="AD9" s="149"/>
+      <c r="AE9" s="149"/>
+      <c r="AF9" s="149"/>
     </row>
     <row r="10" spans="1:32" s="145" customFormat="1">
-      <c r="G10" s="227"/>
-      <c r="H10" s="227"/>
-      <c r="I10" s="227"/>
-      <c r="J10" s="227"/>
-      <c r="K10" s="227"/>
-      <c r="L10" s="227"/>
-      <c r="M10" s="227"/>
-      <c r="N10" s="227"/>
-      <c r="O10" s="227"/>
-      <c r="P10" s="227"/>
-      <c r="Q10" s="227"/>
-      <c r="R10" s="227"/>
-      <c r="S10" s="227"/>
-      <c r="T10" s="227"/>
-      <c r="U10" s="227"/>
-      <c r="V10" s="227"/>
-      <c r="W10" s="227"/>
-      <c r="X10" s="227"/>
-      <c r="Y10" s="227"/>
-      <c r="Z10" s="227"/>
-      <c r="AA10" s="227"/>
-      <c r="AB10" s="227"/>
-      <c r="AC10" s="227"/>
-      <c r="AD10" s="227"/>
-      <c r="AE10" s="227"/>
-      <c r="AF10" s="227"/>
+      <c r="G10" s="149"/>
+      <c r="H10" s="228"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
+      <c r="K10" s="149"/>
+      <c r="L10" s="149"/>
+      <c r="M10" s="149"/>
+      <c r="N10" s="149"/>
+      <c r="O10" s="149"/>
+      <c r="P10" s="149"/>
+      <c r="Q10" s="149"/>
+      <c r="R10" s="149"/>
+      <c r="S10" s="149"/>
+      <c r="T10" s="149"/>
+      <c r="U10" s="149"/>
+      <c r="V10" s="149"/>
+      <c r="W10" s="149"/>
+      <c r="X10" s="149"/>
+      <c r="Y10" s="149"/>
+      <c r="Z10" s="149"/>
+      <c r="AA10" s="149"/>
+      <c r="AB10" s="149"/>
+      <c r="AC10" s="149"/>
+      <c r="AD10" s="149"/>
+      <c r="AE10" s="149"/>
+      <c r="AF10" s="149"/>
     </row>
     <row r="11" spans="1:32" s="141" customFormat="1"/>
     <row r="12" spans="1:32">
@@ -80916,11 +80919,11 @@
       <c r="Z12" s="106"/>
       <c r="AA12" s="106"/>
       <c r="AB12" s="106"/>
-      <c r="AC12" s="164" t="s">
+      <c r="AC12" s="199" t="s">
         <v>318</v>
       </c>
-      <c r="AD12" s="164"/>
-      <c r="AE12" s="164"/>
+      <c r="AD12" s="199"/>
+      <c r="AE12" s="199"/>
       <c r="AF12" s="106"/>
     </row>
     <row r="13" spans="1:32">
@@ -80937,13 +80940,13 @@
       <c r="L13" s="107"/>
       <c r="M13" s="107"/>
       <c r="N13" s="107"/>
-      <c r="O13" s="163" t="s">
+      <c r="O13" s="200" t="s">
         <v>309</v>
       </c>
-      <c r="P13" s="163"/>
-      <c r="Q13" s="163"/>
-      <c r="R13" s="163"/>
-      <c r="S13" s="163"/>
+      <c r="P13" s="200"/>
+      <c r="Q13" s="200"/>
+      <c r="R13" s="200"/>
+      <c r="S13" s="200"/>
       <c r="T13" s="107"/>
       <c r="U13" s="107"/>
       <c r="V13" s="107"/>
@@ -80953,11 +80956,11 @@
       <c r="Z13" s="107"/>
       <c r="AA13" s="106"/>
       <c r="AB13" s="107"/>
-      <c r="AC13" s="165" t="s">
+      <c r="AC13" s="201" t="s">
         <v>319</v>
       </c>
-      <c r="AD13" s="165"/>
-      <c r="AE13" s="165"/>
+      <c r="AD13" s="201"/>
+      <c r="AE13" s="201"/>
       <c r="AF13" s="107"/>
     </row>
     <row r="14" spans="1:32">
@@ -81063,13 +81066,13 @@
       <c r="L17" s="107"/>
       <c r="M17" s="107"/>
       <c r="N17" s="107"/>
-      <c r="O17" s="163" t="s">
+      <c r="O17" s="200" t="s">
         <v>313</v>
       </c>
-      <c r="P17" s="163"/>
-      <c r="Q17" s="163"/>
-      <c r="R17" s="163"/>
-      <c r="S17" s="163"/>
+      <c r="P17" s="200"/>
+      <c r="Q17" s="200"/>
+      <c r="R17" s="200"/>
+      <c r="S17" s="200"/>
       <c r="T17" s="107"/>
       <c r="U17" s="107"/>
       <c r="V17" s="107"/>
@@ -81079,17 +81082,17 @@
       <c r="Z17" s="107"/>
       <c r="AA17" s="106"/>
       <c r="AB17" s="107"/>
-      <c r="AC17" s="163" t="s">
+      <c r="AC17" s="200" t="s">
         <v>314</v>
       </c>
-      <c r="AD17" s="163"/>
-      <c r="AE17" s="163"/>
+      <c r="AD17" s="200"/>
+      <c r="AE17" s="200"/>
       <c r="AF17" s="107"/>
     </row>
     <row r="21" spans="5:32">
-      <c r="AC21" s="200"/>
-      <c r="AD21" s="200"/>
-      <c r="AE21" s="200"/>
+      <c r="AC21" s="198"/>
+      <c r="AD21" s="198"/>
+      <c r="AE21" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -81136,10 +81139,10 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="201" t="s">
+      <c r="L6" s="202" t="s">
         <v>280</v>
       </c>
-      <c r="M6" s="201"/>
+      <c r="M6" s="202"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>

</xml_diff>

<commit_message>
fix: add new mission and new flighter
</commit_message>
<xml_diff>
--- a/xlsx_template/data_template.xlsx
+++ b/xlsx_template/data_template.xlsx
@@ -3428,7 +3428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="237">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3748,16 +3748,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3772,22 +3788,7 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3802,10 +3803,25 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3817,13 +3833,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3831,15 +3841,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3849,21 +3850,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3880,7 +3866,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3889,20 +3881,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3926,6 +3915,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -5211,13 +5212,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>123824</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -8379,17 +8380,17 @@
       <c r="C2" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="E2" s="217" t="s">
+      <c r="E2" s="218" t="s">
         <v>307</v>
       </c>
-      <c r="F2" s="217"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="217"/>
-      <c r="I2" s="217"/>
-      <c r="L2" s="218" t="s">
+      <c r="F2" s="218"/>
+      <c r="G2" s="218"/>
+      <c r="H2" s="218"/>
+      <c r="I2" s="218"/>
+      <c r="L2" s="219" t="s">
         <v>306</v>
       </c>
-      <c r="M2" s="219"/>
+      <c r="M2" s="220"/>
     </row>
     <row r="3" spans="2:13" ht="19.5" customHeight="1">
       <c r="D3" s="131"/>
@@ -8404,30 +8405,30 @@
     </row>
     <row r="4" spans="2:13" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="5" spans="2:13" ht="15.75" thickTop="1">
-      <c r="B5" s="227" t="s">
+      <c r="B5" s="228" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="226" t="s">
+      <c r="C5" s="227" t="s">
         <v>284</v>
       </c>
-      <c r="D5" s="222" t="s">
+      <c r="D5" s="223" t="s">
         <v>286</v>
       </c>
-      <c r="E5" s="222"/>
-      <c r="F5" s="222"/>
-      <c r="G5" s="222"/>
-      <c r="H5" s="222"/>
-      <c r="I5" s="222"/>
-      <c r="J5" s="222"/>
-      <c r="K5" s="222"/>
-      <c r="L5" s="222"/>
-      <c r="M5" s="228" t="s">
+      <c r="E5" s="223"/>
+      <c r="F5" s="223"/>
+      <c r="G5" s="223"/>
+      <c r="H5" s="223"/>
+      <c r="I5" s="223"/>
+      <c r="J5" s="223"/>
+      <c r="K5" s="223"/>
+      <c r="L5" s="223"/>
+      <c r="M5" s="229" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="6" spans="2:13">
-      <c r="B6" s="223"/>
-      <c r="C6" s="224"/>
+      <c r="B6" s="224"/>
+      <c r="C6" s="225"/>
       <c r="D6" s="136" t="s">
         <v>157</v>
       </c>
@@ -8455,21 +8456,21 @@
       <c r="L6" s="137" t="s">
         <v>153</v>
       </c>
-      <c r="M6" s="229"/>
+      <c r="M6" s="230"/>
     </row>
     <row r="7" spans="2:13" ht="10.5" customHeight="1">
-      <c r="B7" s="223"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
-      <c r="L7" s="224"/>
-      <c r="M7" s="225"/>
+      <c r="B7" s="224"/>
+      <c r="C7" s="225"/>
+      <c r="D7" s="225"/>
+      <c r="E7" s="225"/>
+      <c r="F7" s="225"/>
+      <c r="G7" s="225"/>
+      <c r="H7" s="225"/>
+      <c r="I7" s="225"/>
+      <c r="J7" s="225"/>
+      <c r="K7" s="225"/>
+      <c r="L7" s="225"/>
+      <c r="M7" s="226"/>
     </row>
     <row r="8" spans="2:13" s="3" customFormat="1" ht="14.25">
       <c r="B8" s="27" t="s">
@@ -12125,11 +12126,11 @@
     </row>
     <row r="85" spans="1:14" ht="15.75" thickTop="1">
       <c r="C85" s="18"/>
-      <c r="K85" s="220" t="s">
+      <c r="K85" s="221" t="s">
         <v>310</v>
       </c>
-      <c r="L85" s="220"/>
-      <c r="M85" s="220"/>
+      <c r="L85" s="221"/>
+      <c r="M85" s="221"/>
     </row>
     <row r="86" spans="1:14" ht="61.5" customHeight="1">
       <c r="A86" s="3"/>
@@ -12139,18 +12140,18 @@
       </c>
       <c r="D86" s="130"/>
       <c r="E86" s="130"/>
-      <c r="F86" s="221" t="s">
+      <c r="F86" s="222" t="s">
         <v>309</v>
       </c>
-      <c r="G86" s="221"/>
-      <c r="H86" s="221"/>
+      <c r="G86" s="222"/>
+      <c r="H86" s="222"/>
       <c r="I86" s="130"/>
       <c r="J86" s="130"/>
-      <c r="K86" s="217" t="s">
+      <c r="K86" s="218" t="s">
         <v>311</v>
       </c>
-      <c r="L86" s="217"/>
-      <c r="M86" s="217"/>
+      <c r="L86" s="218"/>
+      <c r="M86" s="218"/>
       <c r="N86" s="3"/>
     </row>
     <row r="87" spans="1:14">
@@ -12193,18 +12194,18 @@
       </c>
       <c r="D89" s="130"/>
       <c r="E89" s="130"/>
-      <c r="F89" s="221" t="s">
+      <c r="F89" s="222" t="s">
         <v>313</v>
       </c>
-      <c r="G89" s="221"/>
-      <c r="H89" s="221"/>
+      <c r="G89" s="222"/>
+      <c r="H89" s="222"/>
       <c r="I89" s="130"/>
       <c r="J89" s="130"/>
-      <c r="K89" s="221" t="s">
+      <c r="K89" s="222" t="s">
         <v>314</v>
       </c>
-      <c r="L89" s="221"/>
-      <c r="M89" s="221"/>
+      <c r="L89" s="222"/>
+      <c r="M89" s="222"/>
       <c r="N89" s="3"/>
     </row>
   </sheetData>
@@ -12259,19 +12260,19 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="40"/>
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="203" t="s">
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="201" t="s">
         <v>282</v>
       </c>
-      <c r="F2" s="203"/>
-      <c r="G2" s="203"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="203"/>
-      <c r="J2" s="203"/>
+      <c r="F2" s="201"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="201"/>
+      <c r="J2" s="201"/>
       <c r="K2" s="116"/>
       <c r="L2" s="116"/>
       <c r="M2" s="40"/>
@@ -12306,90 +12307,90 @@
       <c r="H4" s="40"/>
       <c r="I4" s="40"/>
       <c r="J4" s="40"/>
-      <c r="K4" s="205" t="s">
+      <c r="K4" s="214" t="s">
         <v>473</v>
       </c>
-      <c r="L4" s="205"/>
-      <c r="M4" s="205"/>
+      <c r="L4" s="214"/>
+      <c r="M4" s="214"/>
       <c r="N4" s="40"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickTop="1">
       <c r="A5" s="40"/>
-      <c r="B5" s="211" t="s">
+      <c r="B5" s="208" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="213" t="s">
+      <c r="C5" s="210" t="s">
         <v>262</v>
       </c>
-      <c r="D5" s="200" t="s">
+      <c r="D5" s="196" t="s">
         <v>263</v>
       </c>
-      <c r="E5" s="215" t="s">
+      <c r="E5" s="212" t="s">
         <v>264</v>
       </c>
-      <c r="F5" s="215"/>
-      <c r="G5" s="215" t="s">
+      <c r="F5" s="212"/>
+      <c r="G5" s="212" t="s">
         <v>267</v>
       </c>
-      <c r="H5" s="215"/>
-      <c r="I5" s="215"/>
-      <c r="J5" s="215"/>
-      <c r="K5" s="215" t="s">
+      <c r="H5" s="212"/>
+      <c r="I5" s="212"/>
+      <c r="J5" s="212"/>
+      <c r="K5" s="212" t="s">
         <v>272</v>
       </c>
-      <c r="L5" s="215"/>
-      <c r="M5" s="215"/>
-      <c r="N5" s="216"/>
+      <c r="L5" s="212"/>
+      <c r="M5" s="212"/>
+      <c r="N5" s="213"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="40"/>
-      <c r="B6" s="212"/>
-      <c r="C6" s="214"/>
-      <c r="D6" s="194"/>
-      <c r="E6" s="209" t="s">
+      <c r="B6" s="209"/>
+      <c r="C6" s="211"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="206" t="s">
         <v>265</v>
       </c>
-      <c r="F6" s="209" t="s">
+      <c r="F6" s="206" t="s">
         <v>266</v>
       </c>
-      <c r="G6" s="209" t="s">
+      <c r="G6" s="206" t="s">
         <v>268</v>
       </c>
-      <c r="H6" s="209" t="s">
+      <c r="H6" s="206" t="s">
         <v>269</v>
       </c>
-      <c r="I6" s="209" t="s">
+      <c r="I6" s="206" t="s">
         <v>270</v>
       </c>
-      <c r="J6" s="209"/>
-      <c r="K6" s="209" t="s">
+      <c r="J6" s="206"/>
+      <c r="K6" s="206" t="s">
         <v>273</v>
       </c>
-      <c r="L6" s="209" t="s">
+      <c r="L6" s="206" t="s">
         <v>269</v>
       </c>
-      <c r="M6" s="209" t="s">
+      <c r="M6" s="206" t="s">
         <v>270</v>
       </c>
-      <c r="N6" s="210"/>
+      <c r="N6" s="207"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="40"/>
-      <c r="B7" s="212"/>
-      <c r="C7" s="214"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="209"/>
-      <c r="H7" s="209"/>
+      <c r="B7" s="209"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="197"/>
+      <c r="E7" s="206"/>
+      <c r="F7" s="206"/>
+      <c r="G7" s="206"/>
+      <c r="H7" s="206"/>
       <c r="I7" s="155" t="s">
         <v>271</v>
       </c>
       <c r="J7" s="155" t="s">
         <v>141</v>
       </c>
-      <c r="K7" s="209"/>
-      <c r="L7" s="209"/>
+      <c r="K7" s="206"/>
+      <c r="L7" s="206"/>
       <c r="M7" s="155" t="s">
         <v>122</v>
       </c>
@@ -12408,11 +12409,11 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="230" t="s">
+      <c r="K11" s="231" t="s">
         <v>318</v>
       </c>
-      <c r="L11" s="230"/>
-      <c r="M11" s="230"/>
+      <c r="L11" s="231"/>
+      <c r="M11" s="231"/>
       <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14">
@@ -12422,15 +12423,15 @@
       <c r="D12" s="154"/>
       <c r="E12" s="154"/>
       <c r="F12" s="154"/>
-      <c r="G12" s="206"/>
-      <c r="H12" s="206"/>
-      <c r="I12" s="206"/>
+      <c r="G12" s="215"/>
+      <c r="H12" s="215"/>
+      <c r="I12" s="215"/>
       <c r="J12" s="154"/>
-      <c r="K12" s="207" t="s">
+      <c r="K12" s="216" t="s">
         <v>311</v>
       </c>
-      <c r="L12" s="207"/>
-      <c r="M12" s="207"/>
+      <c r="L12" s="216"/>
+      <c r="M12" s="216"/>
       <c r="N12" s="154"/>
     </row>
     <row r="13" spans="1:14">
@@ -12442,11 +12443,11 @@
       <c r="D13" s="154"/>
       <c r="E13" s="154"/>
       <c r="F13" s="154"/>
-      <c r="G13" s="206" t="s">
+      <c r="G13" s="215" t="s">
         <v>309</v>
       </c>
-      <c r="H13" s="206"/>
-      <c r="I13" s="206"/>
+      <c r="H13" s="215"/>
+      <c r="I13" s="215"/>
       <c r="J13" s="154"/>
       <c r="K13" s="154"/>
       <c r="L13" s="154"/>
@@ -12510,17 +12511,17 @@
       <c r="D17" s="154"/>
       <c r="E17" s="154"/>
       <c r="F17" s="154"/>
-      <c r="G17" s="206" t="s">
+      <c r="G17" s="215" t="s">
         <v>313</v>
       </c>
-      <c r="H17" s="206"/>
-      <c r="I17" s="206"/>
+      <c r="H17" s="215"/>
+      <c r="I17" s="215"/>
       <c r="J17" s="154"/>
-      <c r="K17" s="206" t="s">
+      <c r="K17" s="215" t="s">
         <v>314</v>
       </c>
-      <c r="L17" s="206"/>
-      <c r="M17" s="206"/>
+      <c r="L17" s="215"/>
+      <c r="M17" s="215"/>
       <c r="N17" s="10"/>
     </row>
     <row r="18" spans="1:14">
@@ -12541,16 +12542,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="E6:E7"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="K17:M17"/>
     <mergeCell ref="F6:F7"/>
@@ -12564,6 +12555,16 @@
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12626,24 +12627,24 @@
     </row>
     <row r="2" spans="1:32" ht="42.75" customHeight="1">
       <c r="G2" s="21"/>
-      <c r="H2" s="171" t="s">
+      <c r="H2" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="171"/>
-      <c r="J2" s="171"/>
-      <c r="K2" s="171"/>
-      <c r="L2" s="171"/>
-      <c r="M2" s="231" t="s">
+      <c r="I2" s="172"/>
+      <c r="J2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
+      <c r="M2" s="232" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="231"/>
-      <c r="O2" s="231"/>
-      <c r="P2" s="231"/>
-      <c r="Q2" s="231"/>
-      <c r="R2" s="231"/>
-      <c r="S2" s="231"/>
-      <c r="T2" s="231"/>
-      <c r="U2" s="231"/>
+      <c r="N2" s="232"/>
+      <c r="O2" s="232"/>
+      <c r="P2" s="232"/>
+      <c r="Q2" s="232"/>
+      <c r="R2" s="232"/>
+      <c r="S2" s="232"/>
+      <c r="T2" s="232"/>
+      <c r="U2" s="232"/>
       <c r="V2" s="105"/>
       <c r="W2" s="105"/>
       <c r="X2" s="105"/>
@@ -12652,10 +12653,10 @@
       <c r="AA2" s="106"/>
       <c r="AB2" s="106"/>
       <c r="AC2" s="106"/>
-      <c r="AD2" s="172" t="s">
+      <c r="AD2" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="AE2" s="174"/>
+      <c r="AE2" s="175"/>
       <c r="AF2" s="106"/>
     </row>
     <row r="3" spans="1:32" hidden="1">
@@ -12909,11 +12910,11 @@
       <c r="Z12" s="106"/>
       <c r="AA12" s="106"/>
       <c r="AB12" s="106"/>
-      <c r="AC12" s="233" t="s">
+      <c r="AC12" s="234" t="s">
         <v>318</v>
       </c>
-      <c r="AD12" s="233"/>
-      <c r="AE12" s="233"/>
+      <c r="AD12" s="234"/>
+      <c r="AE12" s="234"/>
       <c r="AF12" s="106"/>
     </row>
     <row r="13" spans="1:32">
@@ -12930,13 +12931,13 @@
       <c r="L13" s="107"/>
       <c r="M13" s="107"/>
       <c r="N13" s="107"/>
-      <c r="O13" s="234" t="s">
+      <c r="O13" s="235" t="s">
         <v>309</v>
       </c>
-      <c r="P13" s="234"/>
-      <c r="Q13" s="234"/>
-      <c r="R13" s="234"/>
-      <c r="S13" s="234"/>
+      <c r="P13" s="235"/>
+      <c r="Q13" s="235"/>
+      <c r="R13" s="235"/>
+      <c r="S13" s="235"/>
       <c r="T13" s="107"/>
       <c r="U13" s="107"/>
       <c r="V13" s="107"/>
@@ -12946,11 +12947,11 @@
       <c r="Z13" s="107"/>
       <c r="AA13" s="106"/>
       <c r="AB13" s="107"/>
-      <c r="AC13" s="235" t="s">
+      <c r="AC13" s="236" t="s">
         <v>319</v>
       </c>
-      <c r="AD13" s="235"/>
-      <c r="AE13" s="235"/>
+      <c r="AD13" s="236"/>
+      <c r="AE13" s="236"/>
       <c r="AF13" s="107"/>
     </row>
     <row r="14" spans="1:32">
@@ -13056,13 +13057,13 @@
       <c r="L17" s="107"/>
       <c r="M17" s="107"/>
       <c r="N17" s="107"/>
-      <c r="O17" s="234" t="s">
+      <c r="O17" s="235" t="s">
         <v>313</v>
       </c>
-      <c r="P17" s="234"/>
-      <c r="Q17" s="234"/>
-      <c r="R17" s="234"/>
-      <c r="S17" s="234"/>
+      <c r="P17" s="235"/>
+      <c r="Q17" s="235"/>
+      <c r="R17" s="235"/>
+      <c r="S17" s="235"/>
       <c r="T17" s="107"/>
       <c r="U17" s="107"/>
       <c r="V17" s="107"/>
@@ -13072,17 +13073,17 @@
       <c r="Z17" s="107"/>
       <c r="AA17" s="106"/>
       <c r="AB17" s="107"/>
-      <c r="AC17" s="234" t="s">
+      <c r="AC17" s="235" t="s">
         <v>314</v>
       </c>
-      <c r="AD17" s="234"/>
-      <c r="AE17" s="234"/>
+      <c r="AD17" s="235"/>
+      <c r="AE17" s="235"/>
       <c r="AF17" s="107"/>
     </row>
     <row r="21" spans="5:32">
-      <c r="AC21" s="232"/>
-      <c r="AD21" s="232"/>
-      <c r="AE21" s="232"/>
+      <c r="AC21" s="233"/>
+      <c r="AD21" s="233"/>
+      <c r="AE21" s="233"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -13135,19 +13136,19 @@
         <v>304</v>
       </c>
       <c r="D2" s="127"/>
-      <c r="E2" s="217" t="s">
+      <c r="E2" s="218" t="s">
         <v>307</v>
       </c>
-      <c r="F2" s="217"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="217"/>
-      <c r="I2" s="217"/>
+      <c r="F2" s="218"/>
+      <c r="G2" s="218"/>
+      <c r="H2" s="218"/>
+      <c r="I2" s="218"/>
       <c r="J2" s="127"/>
       <c r="K2" s="127"/>
-      <c r="L2" s="218" t="s">
+      <c r="L2" s="219" t="s">
         <v>306</v>
       </c>
-      <c r="M2" s="219"/>
+      <c r="M2" s="220"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14">
@@ -13186,32 +13187,32 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" thickTop="1">
       <c r="A5" s="7"/>
-      <c r="B5" s="227" t="s">
+      <c r="B5" s="228" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="226" t="s">
+      <c r="C5" s="227" t="s">
         <v>284</v>
       </c>
-      <c r="D5" s="222" t="s">
+      <c r="D5" s="223" t="s">
         <v>286</v>
       </c>
-      <c r="E5" s="222"/>
-      <c r="F5" s="222"/>
-      <c r="G5" s="222"/>
-      <c r="H5" s="222"/>
-      <c r="I5" s="222"/>
-      <c r="J5" s="222"/>
-      <c r="K5" s="222"/>
-      <c r="L5" s="222"/>
-      <c r="M5" s="228" t="s">
+      <c r="E5" s="223"/>
+      <c r="F5" s="223"/>
+      <c r="G5" s="223"/>
+      <c r="H5" s="223"/>
+      <c r="I5" s="223"/>
+      <c r="J5" s="223"/>
+      <c r="K5" s="223"/>
+      <c r="L5" s="223"/>
+      <c r="M5" s="229" t="s">
         <v>285</v>
       </c>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="7"/>
-      <c r="B6" s="223"/>
-      <c r="C6" s="224"/>
+      <c r="B6" s="224"/>
+      <c r="C6" s="225"/>
       <c r="D6" s="136" t="s">
         <v>157</v>
       </c>
@@ -13239,7 +13240,7 @@
       <c r="L6" s="137" t="s">
         <v>153</v>
       </c>
-      <c r="M6" s="229"/>
+      <c r="M6" s="230"/>
       <c r="N6" s="7"/>
     </row>
     <row r="12" spans="1:14">
@@ -13253,11 +13254,11 @@
       <c r="H12" s="127"/>
       <c r="I12" s="127"/>
       <c r="J12" s="127"/>
-      <c r="K12" s="220" t="s">
+      <c r="K12" s="221" t="s">
         <v>310</v>
       </c>
-      <c r="L12" s="220"/>
-      <c r="M12" s="220"/>
+      <c r="L12" s="221"/>
+      <c r="M12" s="221"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="3"/>
@@ -13267,18 +13268,18 @@
       </c>
       <c r="D13" s="130"/>
       <c r="E13" s="130"/>
-      <c r="F13" s="221" t="s">
+      <c r="F13" s="222" t="s">
         <v>309</v>
       </c>
-      <c r="G13" s="221"/>
-      <c r="H13" s="221"/>
+      <c r="G13" s="222"/>
+      <c r="H13" s="222"/>
       <c r="I13" s="130"/>
       <c r="J13" s="130"/>
-      <c r="K13" s="217" t="s">
+      <c r="K13" s="218" t="s">
         <v>311</v>
       </c>
-      <c r="L13" s="217"/>
-      <c r="M13" s="217"/>
+      <c r="L13" s="218"/>
+      <c r="M13" s="218"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="3"/>
@@ -13318,18 +13319,18 @@
       </c>
       <c r="D16" s="130"/>
       <c r="E16" s="130"/>
-      <c r="F16" s="221" t="s">
+      <c r="F16" s="222" t="s">
         <v>313</v>
       </c>
-      <c r="G16" s="221"/>
-      <c r="H16" s="221"/>
+      <c r="G16" s="222"/>
+      <c r="H16" s="222"/>
       <c r="I16" s="130"/>
       <c r="J16" s="130"/>
-      <c r="K16" s="221" t="s">
+      <c r="K16" s="222" t="s">
         <v>314</v>
       </c>
-      <c r="L16" s="221"/>
-      <c r="M16" s="221"/>
+      <c r="L16" s="222"/>
+      <c r="M16" s="222"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="7"/>
@@ -13348,17 +13349,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="K16:M16"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:L5"/>
     <mergeCell ref="M5:M6"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="K16:M16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13376,32 +13377,32 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="41"/>
-      <c r="B1" s="176" t="s">
+      <c r="B1" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183"/>
+      <c r="E1" s="183"/>
+      <c r="F1" s="183"/>
       <c r="G1" s="59"/>
-      <c r="H1" s="176" t="s">
+      <c r="H1" s="178" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+      <c r="M1" s="178"/>
       <c r="N1" s="59"/>
       <c r="O1" s="59"/>
       <c r="P1" s="59"/>
       <c r="Q1" s="59"/>
       <c r="R1" s="89"/>
       <c r="S1" s="89"/>
-      <c r="T1" s="178" t="s">
+      <c r="T1" s="184" t="s">
         <v>167</v>
       </c>
-      <c r="U1" s="179"/>
+      <c r="U1" s="185"/>
       <c r="V1" s="41"/>
       <c r="W1" s="41"/>
     </row>
@@ -13457,7 +13458,7 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" thickTop="1">
       <c r="A4" s="41"/>
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="187" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="180" t="s">
@@ -13491,66 +13492,66 @@
       <c r="U4" s="180" t="s">
         <v>120</v>
       </c>
-      <c r="V4" s="181"/>
+      <c r="V4" s="186"/>
       <c r="W4" s="41"/>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="41"/>
-      <c r="B5" s="184"/>
-      <c r="C5" s="182"/>
-      <c r="D5" s="182" t="s">
+      <c r="B5" s="188"/>
+      <c r="C5" s="181"/>
+      <c r="D5" s="181" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="182" t="s">
+      <c r="E5" s="181" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="182" t="s">
+      <c r="F5" s="181" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="182" t="s">
+      <c r="G5" s="181" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="182" t="s">
+      <c r="H5" s="181" t="s">
         <v>110</v>
       </c>
-      <c r="I5" s="182"/>
-      <c r="J5" s="182" t="s">
+      <c r="I5" s="181"/>
+      <c r="J5" s="181" t="s">
         <v>111</v>
       </c>
-      <c r="K5" s="182"/>
+      <c r="K5" s="181"/>
       <c r="L5" s="152" t="s">
         <v>112</v>
       </c>
-      <c r="M5" s="182" t="s">
+      <c r="M5" s="181" t="s">
         <v>114</v>
       </c>
-      <c r="N5" s="182"/>
-      <c r="O5" s="182"/>
-      <c r="P5" s="182" t="s">
+      <c r="N5" s="181"/>
+      <c r="O5" s="181"/>
+      <c r="P5" s="181" t="s">
         <v>117</v>
       </c>
-      <c r="Q5" s="182"/>
-      <c r="R5" s="182"/>
-      <c r="S5" s="182" t="s">
+      <c r="Q5" s="181"/>
+      <c r="R5" s="181"/>
+      <c r="S5" s="181" t="s">
         <v>112</v>
       </c>
-      <c r="T5" s="182"/>
-      <c r="U5" s="182" t="s">
+      <c r="T5" s="181"/>
+      <c r="U5" s="181" t="s">
         <v>121</v>
       </c>
-      <c r="V5" s="175" t="s">
+      <c r="V5" s="182" t="s">
         <v>122</v>
       </c>
       <c r="W5" s="41"/>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="41"/>
-      <c r="B6" s="184"/>
-      <c r="C6" s="182"/>
-      <c r="D6" s="182"/>
-      <c r="E6" s="182"/>
-      <c r="F6" s="182"/>
-      <c r="G6" s="182"/>
+      <c r="B6" s="188"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="181"/>
+      <c r="G6" s="181"/>
       <c r="H6" s="152" t="s">
         <v>108</v>
       </c>
@@ -13584,10 +13585,10 @@
       <c r="R6" s="152" t="s">
         <v>7</v>
       </c>
-      <c r="S6" s="182"/>
-      <c r="T6" s="182"/>
-      <c r="U6" s="182"/>
-      <c r="V6" s="175"/>
+      <c r="S6" s="181"/>
+      <c r="T6" s="181"/>
+      <c r="U6" s="181"/>
+      <c r="V6" s="182"/>
       <c r="W6" s="41"/>
     </row>
     <row r="9" spans="1:23">
@@ -13793,41 +13794,41 @@
       <c r="P16" s="41"/>
       <c r="Q16" s="41"/>
       <c r="R16" s="41"/>
-      <c r="S16" s="185" t="s">
+      <c r="S16" s="176" t="s">
         <v>318</v>
       </c>
-      <c r="T16" s="185"/>
-      <c r="U16" s="185"/>
+      <c r="T16" s="176"/>
+      <c r="U16" s="176"/>
       <c r="V16" s="41"/>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="91"/>
       <c r="B17" s="151"/>
-      <c r="C17" s="186" t="s">
+      <c r="C17" s="177" t="s">
         <v>308</v>
       </c>
-      <c r="D17" s="186"/>
+      <c r="D17" s="177"/>
       <c r="E17" s="91"/>
       <c r="F17" s="91"/>
       <c r="G17" s="91"/>
       <c r="H17" s="91"/>
       <c r="I17" s="91"/>
       <c r="J17" s="91"/>
-      <c r="K17" s="186" t="s">
+      <c r="K17" s="177" t="s">
         <v>309</v>
       </c>
-      <c r="L17" s="186"/>
-      <c r="M17" s="186"/>
+      <c r="L17" s="177"/>
+      <c r="M17" s="177"/>
       <c r="N17" s="91"/>
       <c r="O17" s="91"/>
       <c r="P17" s="91"/>
       <c r="Q17" s="91"/>
       <c r="R17" s="91"/>
-      <c r="S17" s="187" t="s">
+      <c r="S17" s="179" t="s">
         <v>339</v>
       </c>
-      <c r="T17" s="187"/>
-      <c r="U17" s="187"/>
+      <c r="T17" s="179"/>
+      <c r="U17" s="179"/>
       <c r="V17" s="91"/>
     </row>
     <row r="18" spans="1:22">
@@ -13905,35 +13906,52 @@
     <row r="21" spans="1:22">
       <c r="A21" s="91"/>
       <c r="B21" s="151"/>
-      <c r="C21" s="186" t="s">
+      <c r="C21" s="177" t="s">
         <v>312</v>
       </c>
-      <c r="D21" s="186"/>
+      <c r="D21" s="177"/>
       <c r="E21" s="91"/>
       <c r="F21" s="91"/>
       <c r="G21" s="91"/>
       <c r="H21" s="91"/>
       <c r="I21" s="91"/>
       <c r="J21" s="91"/>
-      <c r="K21" s="186" t="s">
+      <c r="K21" s="177" t="s">
         <v>313</v>
       </c>
-      <c r="L21" s="186"/>
-      <c r="M21" s="186"/>
+      <c r="L21" s="177"/>
+      <c r="M21" s="177"/>
       <c r="N21" s="91"/>
       <c r="O21" s="91"/>
       <c r="P21" s="91"/>
       <c r="Q21" s="91"/>
       <c r="R21" s="91"/>
-      <c r="S21" s="186" t="s">
+      <c r="S21" s="177" t="s">
         <v>314</v>
       </c>
-      <c r="T21" s="186"/>
-      <c r="U21" s="186"/>
+      <c r="T21" s="177"/>
+      <c r="U21" s="177"/>
       <c r="V21" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="U5:U6"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="T1:U1"/>
@@ -13945,23 +13963,6 @@
     <mergeCell ref="T4:T6"/>
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="V5:V6"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="S21:U21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13969,42 +13970,43 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE18"/>
+  <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="153"/>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="153"/>
+    <col min="2" max="2" width="0" style="153" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="0" style="157" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:31">
-      <c r="C1" s="153"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="153"/>
+    <row r="1" spans="3:32">
+      <c r="D1" s="153"/>
+      <c r="E1" s="39"/>
       <c r="F1" s="153"/>
       <c r="G1" s="153"/>
       <c r="H1" s="153"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="153"/>
+      <c r="I1" s="153"/>
+      <c r="J1" s="70"/>
       <c r="K1" s="153"/>
       <c r="L1" s="153"/>
-      <c r="M1" s="70"/>
+      <c r="M1" s="153"/>
       <c r="N1" s="70"/>
       <c r="O1" s="70"/>
       <c r="P1" s="70"/>
       <c r="Q1" s="70"/>
-      <c r="R1" s="153"/>
+      <c r="R1" s="70"/>
       <c r="S1" s="153"/>
       <c r="T1" s="153"/>
       <c r="U1" s="153"/>
-      <c r="V1" s="45"/>
+      <c r="V1" s="153"/>
       <c r="W1" s="45"/>
-      <c r="X1" s="153"/>
+      <c r="X1" s="45"/>
       <c r="Y1" s="153"/>
       <c r="Z1" s="153"/>
       <c r="AA1" s="153"/>
@@ -14012,67 +14014,67 @@
       <c r="AC1" s="153"/>
       <c r="AD1" s="153"/>
       <c r="AE1" s="153"/>
-    </row>
-    <row r="2" spans="3:31" ht="31.5" customHeight="1">
-      <c r="C2" s="44"/>
-      <c r="D2" s="203" t="s">
+      <c r="AF1" s="153"/>
+    </row>
+    <row r="2" spans="3:32" ht="31.5" customHeight="1">
+      <c r="D2" s="44"/>
+      <c r="E2" s="201" t="s">
         <v>163</v>
       </c>
-      <c r="E2" s="203"/>
-      <c r="F2" s="203"/>
-      <c r="G2" s="203"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="203"/>
-      <c r="J2" s="203"/>
-      <c r="K2" s="236" t="s">
+      <c r="F2" s="201"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="201"/>
+      <c r="J2" s="201"/>
+      <c r="K2" s="201"/>
+      <c r="L2" s="237" t="s">
         <v>999</v>
       </c>
-      <c r="L2" s="236"/>
-      <c r="M2" s="236"/>
-      <c r="N2" s="236"/>
-      <c r="O2" s="236"/>
-      <c r="P2" s="236"/>
-      <c r="Q2" s="236"/>
-      <c r="R2" s="236"/>
-      <c r="S2" s="236"/>
-      <c r="T2" s="236"/>
-      <c r="U2" s="236"/>
-      <c r="V2" s="43"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237"/>
+      <c r="O2" s="237"/>
+      <c r="P2" s="237"/>
+      <c r="Q2" s="237"/>
+      <c r="R2" s="237"/>
+      <c r="S2" s="237"/>
+      <c r="T2" s="237"/>
+      <c r="U2" s="237"/>
+      <c r="V2" s="237"/>
       <c r="W2" s="43"/>
-      <c r="X2" s="44"/>
+      <c r="X2" s="43"/>
       <c r="Y2" s="44"/>
       <c r="Z2" s="44"/>
-      <c r="AA2" s="196" t="s">
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="192" t="s">
         <v>143</v>
       </c>
-      <c r="AB2" s="197"/>
-      <c r="AC2" s="44"/>
+      <c r="AC2" s="193"/>
       <c r="AD2" s="44"/>
       <c r="AE2" s="44"/>
-    </row>
-    <row r="3" spans="3:31">
-      <c r="C3" s="153"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="153"/>
+      <c r="AF2" s="44"/>
+    </row>
+    <row r="3" spans="3:32">
+      <c r="D3" s="153"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="153"/>
       <c r="G3" s="153"/>
       <c r="H3" s="153"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="70"/>
       <c r="K3" s="153"/>
       <c r="L3" s="153"/>
-      <c r="M3" s="70"/>
+      <c r="M3" s="153"/>
       <c r="N3" s="70"/>
       <c r="O3" s="70"/>
       <c r="P3" s="70"/>
       <c r="Q3" s="70"/>
-      <c r="R3" s="153"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="153"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="153"/>
+      <c r="T3" s="37"/>
       <c r="U3" s="153"/>
-      <c r="V3" s="45"/>
+      <c r="V3" s="153"/>
       <c r="W3" s="45"/>
-      <c r="X3" s="153"/>
+      <c r="X3" s="45"/>
       <c r="Y3" s="153"/>
       <c r="Z3" s="153"/>
       <c r="AA3" s="153"/>
@@ -14080,459 +14082,466 @@
       <c r="AC3" s="153"/>
       <c r="AD3" s="153"/>
       <c r="AE3" s="153"/>
-    </row>
-    <row r="4" spans="3:31" ht="15.75" thickBot="1">
-      <c r="C4" s="153"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="7"/>
+      <c r="AF3" s="153"/>
+    </row>
+    <row r="4" spans="3:32" ht="15.75" thickBot="1">
+      <c r="D4" s="153"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="8"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="7"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="41"/>
       <c r="U4" s="7"/>
-      <c r="V4" s="8"/>
+      <c r="V4" s="7"/>
       <c r="W4" s="8"/>
-      <c r="X4" s="7"/>
+      <c r="X4" s="8"/>
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
-      <c r="AE4" s="153"/>
-    </row>
-    <row r="5" spans="3:31" ht="15.75" thickTop="1">
-      <c r="C5" s="153"/>
-      <c r="D5" s="198" t="s">
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="153"/>
+    </row>
+    <row r="5" spans="3:32" ht="15.75" thickTop="1">
+      <c r="D5" s="153"/>
+      <c r="E5" s="194" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="200" t="s">
+      <c r="F5" s="196" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="200" t="s">
+      <c r="G5" s="196" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="200"/>
-      <c r="H5" s="200"/>
-      <c r="I5" s="200"/>
-      <c r="J5" s="200" t="s">
+      <c r="H5" s="196"/>
+      <c r="I5" s="196"/>
+      <c r="J5" s="196"/>
+      <c r="K5" s="196" t="s">
         <v>131</v>
       </c>
-      <c r="K5" s="200"/>
-      <c r="L5" s="200"/>
-      <c r="M5" s="200" t="s">
+      <c r="L5" s="196"/>
+      <c r="M5" s="196"/>
+      <c r="N5" s="196" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="200"/>
-      <c r="O5" s="200"/>
-      <c r="P5" s="201" t="s">
+      <c r="O5" s="196"/>
+      <c r="P5" s="196"/>
+      <c r="Q5" s="198" t="s">
         <v>134</v>
       </c>
-      <c r="Q5" s="201" t="s">
+      <c r="R5" s="198" t="s">
         <v>135</v>
       </c>
-      <c r="R5" s="200" t="s">
+      <c r="S5" s="196" t="s">
         <v>136</v>
       </c>
-      <c r="S5" s="200"/>
-      <c r="T5" s="200"/>
-      <c r="U5" s="200"/>
-      <c r="V5" s="201" t="s">
+      <c r="T5" s="196"/>
+      <c r="U5" s="196"/>
+      <c r="V5" s="196"/>
+      <c r="W5" s="198" t="s">
         <v>138</v>
       </c>
-      <c r="W5" s="201"/>
-      <c r="X5" s="200" t="s">
+      <c r="X5" s="198"/>
+      <c r="Y5" s="196" t="s">
         <v>139</v>
       </c>
-      <c r="Y5" s="200"/>
-      <c r="Z5" s="200" t="s">
+      <c r="Z5" s="196"/>
+      <c r="AA5" s="196" t="s">
         <v>140</v>
       </c>
-      <c r="AA5" s="200"/>
-      <c r="AB5" s="200"/>
-      <c r="AC5" s="200"/>
-      <c r="AD5" s="192" t="s">
+      <c r="AB5" s="196"/>
+      <c r="AC5" s="196"/>
+      <c r="AD5" s="196"/>
+      <c r="AE5" s="203" t="s">
         <v>142</v>
       </c>
-      <c r="AE5" s="153"/>
-    </row>
-    <row r="6" spans="3:31">
-      <c r="C6" s="153"/>
-      <c r="D6" s="199"/>
-      <c r="E6" s="194"/>
-      <c r="F6" s="194" t="s">
+      <c r="AF5" s="153"/>
+    </row>
+    <row r="6" spans="3:32">
+      <c r="D6" s="153"/>
+      <c r="E6" s="195"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="197" t="s">
         <v>128</v>
       </c>
-      <c r="G6" s="194"/>
-      <c r="H6" s="194"/>
-      <c r="I6" s="195" t="s">
+      <c r="H6" s="197"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="199" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="194" t="s">
+      <c r="K6" s="197" t="s">
         <v>133</v>
       </c>
-      <c r="K6" s="194" t="s">
+      <c r="L6" s="197" t="s">
         <v>132</v>
       </c>
-      <c r="L6" s="194" t="s">
+      <c r="M6" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="195" t="s">
+      <c r="N6" s="199" t="s">
         <v>133</v>
       </c>
-      <c r="N6" s="195" t="s">
+      <c r="O6" s="199" t="s">
         <v>132</v>
       </c>
-      <c r="O6" s="195" t="s">
+      <c r="P6" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="195"/>
-      <c r="Q6" s="195"/>
-      <c r="R6" s="194" t="s">
+      <c r="Q6" s="199"/>
+      <c r="R6" s="199"/>
+      <c r="S6" s="197" t="s">
         <v>128</v>
       </c>
-      <c r="S6" s="194"/>
-      <c r="T6" s="194" t="s">
+      <c r="T6" s="197"/>
+      <c r="U6" s="197" t="s">
         <v>137</v>
       </c>
-      <c r="U6" s="194"/>
-      <c r="V6" s="195" t="s">
+      <c r="V6" s="197"/>
+      <c r="W6" s="199" t="s">
         <v>129</v>
       </c>
-      <c r="W6" s="195" t="s">
+      <c r="X6" s="199" t="s">
         <v>130</v>
       </c>
-      <c r="X6" s="194" t="s">
+      <c r="Y6" s="197" t="s">
         <v>129</v>
       </c>
-      <c r="Y6" s="194" t="s">
+      <c r="Z6" s="197" t="s">
         <v>130</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AA6" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2" t="s">
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="193"/>
-      <c r="AE6" s="153"/>
-    </row>
-    <row r="7" spans="3:31">
-      <c r="C7" s="153"/>
-      <c r="D7" s="199"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="2" t="s">
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="204"/>
+      <c r="AF6" s="153"/>
+    </row>
+    <row r="7" spans="3:32">
+      <c r="D7" s="153"/>
+      <c r="E7" s="195"/>
+      <c r="F7" s="197"/>
+      <c r="G7" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="195"/>
-      <c r="J7" s="194"/>
-      <c r="K7" s="194"/>
-      <c r="L7" s="194"/>
-      <c r="M7" s="195"/>
-      <c r="N7" s="195"/>
-      <c r="O7" s="195"/>
-      <c r="P7" s="195"/>
-      <c r="Q7" s="195"/>
-      <c r="R7" s="2" t="s">
+      <c r="J7" s="199"/>
+      <c r="K7" s="197"/>
+      <c r="L7" s="197"/>
+      <c r="M7" s="197"/>
+      <c r="N7" s="199"/>
+      <c r="O7" s="199"/>
+      <c r="P7" s="199"/>
+      <c r="Q7" s="199"/>
+      <c r="R7" s="199"/>
+      <c r="S7" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="S7" s="42" t="s">
+      <c r="T7" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="U7" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="V7" s="195"/>
-      <c r="W7" s="195"/>
-      <c r="X7" s="194"/>
-      <c r="Y7" s="194"/>
-      <c r="Z7" s="2" t="s">
+      <c r="W7" s="199"/>
+      <c r="X7" s="199"/>
+      <c r="Y7" s="197"/>
+      <c r="Z7" s="197"/>
+      <c r="AA7" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA7" s="2" t="s">
+      <c r="AB7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AB7" s="2" t="s">
+      <c r="AC7" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AC7" s="2" t="s">
+      <c r="AD7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AD7" s="193"/>
-      <c r="AE7" s="153"/>
-    </row>
-    <row r="9" spans="3:31" s="153" customFormat="1"/>
-    <row r="10" spans="3:31" s="153" customFormat="1"/>
-    <row r="11" spans="3:31" s="153" customFormat="1"/>
-    <row r="13" spans="3:31">
-      <c r="C13" s="153"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="153"/>
+      <c r="AE7" s="204"/>
+      <c r="AF7" s="153"/>
+    </row>
+    <row r="9" spans="3:32" s="153" customFormat="1">
+      <c r="C9" s="157"/>
+    </row>
+    <row r="10" spans="3:32" s="153" customFormat="1">
+      <c r="C10" s="157"/>
+    </row>
+    <row r="11" spans="3:32" s="153" customFormat="1">
+      <c r="C11" s="157"/>
+    </row>
+    <row r="13" spans="3:32">
+      <c r="D13" s="153"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="153"/>
       <c r="G13" s="153"/>
       <c r="H13" s="153"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="153"/>
+      <c r="I13" s="153"/>
+      <c r="J13" s="70"/>
       <c r="K13" s="153"/>
       <c r="L13" s="153"/>
-      <c r="M13" s="70"/>
+      <c r="M13" s="153"/>
       <c r="N13" s="70"/>
       <c r="O13" s="70"/>
       <c r="P13" s="70"/>
       <c r="Q13" s="70"/>
-      <c r="R13" s="153"/>
+      <c r="R13" s="70"/>
       <c r="S13" s="153"/>
       <c r="T13" s="153"/>
       <c r="U13" s="153"/>
-      <c r="V13" s="45"/>
+      <c r="V13" s="153"/>
       <c r="W13" s="45"/>
-      <c r="X13" s="153"/>
+      <c r="X13" s="45"/>
       <c r="Y13" s="153"/>
       <c r="Z13" s="153"/>
-      <c r="AA13" s="153" t="s">
+      <c r="AA13" s="153"/>
+      <c r="AB13" s="153" t="s">
         <v>318</v>
       </c>
-      <c r="AB13" s="153"/>
       <c r="AC13" s="153"/>
       <c r="AD13" s="153"/>
-    </row>
-    <row r="14" spans="3:31">
-      <c r="C14" s="5"/>
-      <c r="D14" s="114"/>
-      <c r="E14" s="5" t="s">
+      <c r="AE13" s="153"/>
+    </row>
+    <row r="14" spans="3:32">
+      <c r="D14" s="5"/>
+      <c r="E14" s="114"/>
+      <c r="F14" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="169" t="s">
+      <c r="H14" s="5"/>
+      <c r="I14" s="162" t="s">
         <v>463</v>
       </c>
-      <c r="I14" s="169"/>
-      <c r="J14" s="5"/>
+      <c r="J14" s="162"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="169" t="s">
+      <c r="L14" s="5"/>
+      <c r="M14" s="162" t="s">
         <v>465</v>
       </c>
-      <c r="M14" s="169"/>
-      <c r="N14" s="169"/>
-      <c r="O14" s="115"/>
+      <c r="N14" s="162"/>
+      <c r="O14" s="162"/>
       <c r="P14" s="115"/>
-      <c r="Q14" s="191" t="s">
+      <c r="Q14" s="115"/>
+      <c r="R14" s="202" t="s">
         <v>467</v>
       </c>
-      <c r="R14" s="191"/>
-      <c r="S14" s="191"/>
-      <c r="T14" s="5"/>
+      <c r="S14" s="202"/>
+      <c r="T14" s="202"/>
       <c r="U14" s="5"/>
-      <c r="V14" s="191" t="s">
+      <c r="V14" s="5"/>
+      <c r="W14" s="202" t="s">
         <v>469</v>
       </c>
-      <c r="W14" s="191"/>
-      <c r="X14" s="191"/>
-      <c r="Y14" s="5"/>
+      <c r="X14" s="202"/>
+      <c r="Y14" s="202"/>
       <c r="Z14" s="5"/>
-      <c r="AA14" s="169" t="s">
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="162" t="s">
         <v>471</v>
       </c>
-      <c r="AB14" s="169"/>
-      <c r="AC14" s="169"/>
-      <c r="AD14" s="5"/>
-    </row>
-    <row r="15" spans="3:31">
-      <c r="C15" s="153"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="153"/>
+      <c r="AC14" s="162"/>
+      <c r="AD14" s="162"/>
+      <c r="AE14" s="5"/>
+    </row>
+    <row r="15" spans="3:32">
+      <c r="D15" s="153"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="153"/>
       <c r="G15" s="153"/>
       <c r="H15" s="153"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="153"/>
+      <c r="I15" s="153"/>
+      <c r="J15" s="70"/>
       <c r="K15" s="153"/>
       <c r="L15" s="153"/>
-      <c r="M15" s="70"/>
+      <c r="M15" s="153"/>
       <c r="N15" s="70"/>
       <c r="O15" s="70"/>
       <c r="P15" s="70"/>
       <c r="Q15" s="70"/>
-      <c r="R15" s="153"/>
+      <c r="R15" s="70"/>
       <c r="S15" s="153"/>
       <c r="T15" s="153"/>
       <c r="U15" s="153"/>
-      <c r="V15" s="45"/>
+      <c r="V15" s="153"/>
       <c r="W15" s="45"/>
-      <c r="X15" s="153"/>
+      <c r="X15" s="45"/>
       <c r="Y15" s="153"/>
       <c r="Z15" s="153"/>
       <c r="AA15" s="153"/>
       <c r="AB15" s="153"/>
       <c r="AC15" s="153"/>
       <c r="AD15" s="153"/>
-    </row>
-    <row r="16" spans="3:31">
-      <c r="C16" s="153"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="153"/>
+      <c r="AE15" s="153"/>
+    </row>
+    <row r="16" spans="3:32">
+      <c r="D16" s="153"/>
+      <c r="E16" s="39"/>
       <c r="F16" s="153"/>
       <c r="G16" s="153"/>
       <c r="H16" s="153"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="153"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="70"/>
       <c r="K16" s="153"/>
       <c r="L16" s="153"/>
-      <c r="M16" s="70"/>
+      <c r="M16" s="153"/>
       <c r="N16" s="70"/>
       <c r="O16" s="70"/>
       <c r="P16" s="70"/>
       <c r="Q16" s="70"/>
-      <c r="R16" s="153"/>
+      <c r="R16" s="70"/>
       <c r="S16" s="153"/>
       <c r="T16" s="153"/>
       <c r="U16" s="153"/>
-      <c r="V16" s="45"/>
+      <c r="V16" s="153"/>
       <c r="W16" s="45"/>
-      <c r="X16" s="153"/>
+      <c r="X16" s="45"/>
       <c r="Y16" s="153"/>
       <c r="Z16" s="153"/>
       <c r="AA16" s="153"/>
       <c r="AB16" s="153"/>
       <c r="AC16" s="153"/>
       <c r="AD16" s="153"/>
-    </row>
-    <row r="17" spans="3:30">
-      <c r="C17" s="153"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="153"/>
+      <c r="AE16" s="153"/>
+    </row>
+    <row r="17" spans="4:31">
+      <c r="D17" s="153"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="153"/>
       <c r="G17" s="153"/>
       <c r="H17" s="153"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="153"/>
+      <c r="I17" s="153"/>
+      <c r="J17" s="70"/>
       <c r="K17" s="153"/>
       <c r="L17" s="153"/>
-      <c r="M17" s="70"/>
+      <c r="M17" s="153"/>
       <c r="N17" s="70"/>
       <c r="O17" s="70"/>
       <c r="P17" s="70"/>
       <c r="Q17" s="70"/>
-      <c r="R17" s="153"/>
+      <c r="R17" s="70"/>
       <c r="S17" s="153"/>
       <c r="T17" s="153"/>
       <c r="U17" s="153"/>
-      <c r="V17" s="45"/>
+      <c r="V17" s="153"/>
       <c r="W17" s="45"/>
-      <c r="X17" s="153"/>
+      <c r="X17" s="45"/>
       <c r="Y17" s="153"/>
       <c r="Z17" s="153"/>
       <c r="AA17" s="153"/>
       <c r="AB17" s="153"/>
       <c r="AC17" s="153"/>
       <c r="AD17" s="153"/>
-    </row>
-    <row r="18" spans="3:30">
-      <c r="C18" s="5"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="5" t="s">
+      <c r="AE17" s="153"/>
+    </row>
+    <row r="18" spans="4:31">
+      <c r="D18" s="5"/>
+      <c r="E18" s="114"/>
+      <c r="F18" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="169" t="s">
+      <c r="H18" s="5"/>
+      <c r="I18" s="162" t="s">
         <v>464</v>
       </c>
-      <c r="I18" s="169"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="169" t="s">
+      <c r="J18" s="162"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="162" t="s">
         <v>466</v>
       </c>
-      <c r="M18" s="169"/>
-      <c r="N18" s="169"/>
-      <c r="O18" s="115"/>
+      <c r="N18" s="162"/>
+      <c r="O18" s="162"/>
       <c r="P18" s="115"/>
-      <c r="Q18" s="191" t="s">
+      <c r="Q18" s="115"/>
+      <c r="R18" s="202" t="s">
         <v>468</v>
       </c>
-      <c r="R18" s="191"/>
-      <c r="S18" s="191"/>
-      <c r="T18" s="5"/>
+      <c r="S18" s="202"/>
+      <c r="T18" s="202"/>
       <c r="U18" s="5"/>
-      <c r="V18" s="191" t="s">
+      <c r="V18" s="5"/>
+      <c r="W18" s="202" t="s">
         <v>470</v>
       </c>
-      <c r="W18" s="191"/>
-      <c r="X18" s="191"/>
-      <c r="Y18" s="5"/>
+      <c r="X18" s="202"/>
+      <c r="Y18" s="202"/>
       <c r="Z18" s="5"/>
-      <c r="AA18" s="169" t="s">
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="162" t="s">
         <v>472</v>
       </c>
-      <c r="AB18" s="169"/>
-      <c r="AC18" s="169"/>
-      <c r="AD18" s="5"/>
+      <c r="AC18" s="162"/>
+      <c r="AD18" s="162"/>
+      <c r="AE18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="AA14:AC14"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="V18:X18"/>
-    <mergeCell ref="AA18:AC18"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="V14:X14"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="Q5:Q7"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="K2:U2"/>
-    <mergeCell ref="AD5:AD7"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="AE5:AE7"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
-    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="M6:M7"/>
     <mergeCell ref="X6:X7"/>
     <mergeCell ref="Y6:Y7"/>
-    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="Z6:Z7"/>
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="O6:O7"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:Q7"/>
+    <mergeCell ref="R5:R7"/>
+    <mergeCell ref="S5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="L2:V2"/>
+    <mergeCell ref="AB14:AD14"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="AB18:AD18"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="W14:Y14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14843,163 +14852,163 @@
       <c r="F2" s="66"/>
       <c r="G2" s="66"/>
       <c r="H2" s="66"/>
-      <c r="I2" s="169" t="s">
+      <c r="I2" s="162" t="s">
         <v>215</v>
       </c>
-      <c r="J2" s="169"/>
-      <c r="K2" s="169"/>
-      <c r="L2" s="169"/>
-      <c r="M2" s="169"/>
-      <c r="N2" s="169"/>
-      <c r="O2" s="169"/>
-      <c r="P2" s="169"/>
-      <c r="Q2" s="169"/>
-      <c r="R2" s="169"/>
-      <c r="S2" s="169"/>
-      <c r="T2" s="169"/>
-      <c r="U2" s="169"/>
-      <c r="V2" s="169"/>
-      <c r="W2" s="169"/>
-      <c r="X2" s="169"/>
-      <c r="Y2" s="169"/>
-      <c r="Z2" s="169"/>
+      <c r="J2" s="162"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="162"/>
+      <c r="M2" s="162"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="162"/>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+      <c r="R2" s="162"/>
+      <c r="S2" s="162"/>
+      <c r="T2" s="162"/>
+      <c r="U2" s="162"/>
+      <c r="V2" s="162"/>
+      <c r="W2" s="162"/>
+      <c r="X2" s="162"/>
+      <c r="Y2" s="162"/>
+      <c r="Z2" s="162"/>
     </row>
     <row r="5" spans="2:34">
-      <c r="D5" s="161" t="s">
+      <c r="D5" s="167" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="159" t="s">
+      <c r="E5" s="158" t="s">
         <v>217</v>
       </c>
-      <c r="F5" s="165" t="s">
+      <c r="F5" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="166"/>
-      <c r="H5" s="165" t="s">
+      <c r="G5" s="161"/>
+      <c r="H5" s="160" t="s">
         <v>229</v>
       </c>
-      <c r="I5" s="167"/>
-      <c r="J5" s="167"/>
-      <c r="K5" s="167"/>
-      <c r="L5" s="167"/>
-      <c r="M5" s="167"/>
-      <c r="N5" s="167"/>
-      <c r="O5" s="166"/>
-      <c r="P5" s="165" t="s">
+      <c r="I5" s="171"/>
+      <c r="J5" s="171"/>
+      <c r="K5" s="171"/>
+      <c r="L5" s="171"/>
+      <c r="M5" s="171"/>
+      <c r="N5" s="171"/>
+      <c r="O5" s="161"/>
+      <c r="P5" s="160" t="s">
         <v>228</v>
       </c>
-      <c r="Q5" s="167"/>
-      <c r="R5" s="167"/>
-      <c r="S5" s="167"/>
-      <c r="T5" s="167"/>
-      <c r="U5" s="167"/>
-      <c r="V5" s="166"/>
-      <c r="W5" s="165" t="s">
+      <c r="Q5" s="171"/>
+      <c r="R5" s="171"/>
+      <c r="S5" s="171"/>
+      <c r="T5" s="171"/>
+      <c r="U5" s="171"/>
+      <c r="V5" s="161"/>
+      <c r="W5" s="160" t="s">
         <v>135</v>
       </c>
-      <c r="X5" s="166"/>
-      <c r="Y5" s="170" t="s">
+      <c r="X5" s="161"/>
+      <c r="Y5" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="Z5" s="170"/>
+      <c r="Z5" s="165"/>
       <c r="AA5" s="75"/>
       <c r="AB5" s="75"/>
     </row>
     <row r="6" spans="2:34" ht="15" customHeight="1">
-      <c r="D6" s="162"/>
-      <c r="E6" s="164"/>
-      <c r="F6" s="159" t="s">
+      <c r="D6" s="168"/>
+      <c r="E6" s="170"/>
+      <c r="F6" s="158" t="s">
         <v>218</v>
       </c>
-      <c r="G6" s="159" t="s">
+      <c r="G6" s="158" t="s">
         <v>219</v>
       </c>
-      <c r="H6" s="159" t="s">
+      <c r="H6" s="158" t="s">
         <v>220</v>
       </c>
-      <c r="I6" s="159" t="s">
+      <c r="I6" s="158" t="s">
         <v>221</v>
       </c>
-      <c r="J6" s="159" t="s">
+      <c r="J6" s="158" t="s">
         <v>222</v>
       </c>
-      <c r="K6" s="157" t="s">
+      <c r="K6" s="163" t="s">
         <v>223</v>
       </c>
-      <c r="L6" s="159" t="s">
+      <c r="L6" s="158" t="s">
         <v>230</v>
       </c>
-      <c r="M6" s="159" t="s">
+      <c r="M6" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="168" t="s">
+      <c r="N6" s="166" t="s">
         <v>135</v>
       </c>
-      <c r="O6" s="168"/>
-      <c r="P6" s="157" t="s">
+      <c r="O6" s="166"/>
+      <c r="P6" s="163" t="s">
         <v>224</v>
       </c>
-      <c r="Q6" s="159" t="s">
+      <c r="Q6" s="158" t="s">
         <v>225</v>
       </c>
-      <c r="R6" s="159" t="s">
+      <c r="R6" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="S6" s="157" t="s">
+      <c r="S6" s="163" t="s">
         <v>226</v>
       </c>
-      <c r="T6" s="157" t="s">
+      <c r="T6" s="163" t="s">
         <v>231</v>
       </c>
-      <c r="U6" s="157" t="s">
+      <c r="U6" s="163" t="s">
         <v>12</v>
       </c>
-      <c r="V6" s="159" t="s">
+      <c r="V6" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="W6" s="159" t="s">
+      <c r="W6" s="158" t="s">
         <v>227</v>
       </c>
-      <c r="X6" s="159" t="s">
+      <c r="X6" s="158" t="s">
         <v>219</v>
       </c>
-      <c r="Y6" s="168" t="s">
+      <c r="Y6" s="166" t="s">
         <v>218</v>
       </c>
-      <c r="Z6" s="168" t="s">
+      <c r="Z6" s="166" t="s">
         <v>219</v>
       </c>
       <c r="AA6" s="76"/>
       <c r="AB6" s="76"/>
     </row>
     <row r="7" spans="2:34">
-      <c r="D7" s="163"/>
-      <c r="E7" s="160"/>
-      <c r="F7" s="160"/>
-      <c r="G7" s="160"/>
-      <c r="H7" s="160"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="160"/>
-      <c r="K7" s="158"/>
-      <c r="L7" s="160"/>
-      <c r="M7" s="160"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="159"/>
+      <c r="F7" s="159"/>
+      <c r="G7" s="159"/>
+      <c r="H7" s="159"/>
+      <c r="I7" s="159"/>
+      <c r="J7" s="159"/>
+      <c r="K7" s="164"/>
+      <c r="L7" s="159"/>
+      <c r="M7" s="159"/>
       <c r="N7" s="77" t="s">
         <v>218</v>
       </c>
       <c r="O7" s="71" t="s">
         <v>219</v>
       </c>
-      <c r="P7" s="158"/>
-      <c r="Q7" s="160"/>
-      <c r="R7" s="160"/>
-      <c r="S7" s="158"/>
-      <c r="T7" s="158"/>
-      <c r="U7" s="158"/>
-      <c r="V7" s="160"/>
-      <c r="W7" s="160"/>
-      <c r="X7" s="160"/>
-      <c r="Y7" s="168"/>
-      <c r="Z7" s="168"/>
+      <c r="P7" s="164"/>
+      <c r="Q7" s="159"/>
+      <c r="R7" s="159"/>
+      <c r="S7" s="164"/>
+      <c r="T7" s="164"/>
+      <c r="U7" s="164"/>
+      <c r="V7" s="159"/>
+      <c r="W7" s="159"/>
+      <c r="X7" s="159"/>
+      <c r="Y7" s="166"/>
+      <c r="Z7" s="166"/>
       <c r="AA7" s="76"/>
       <c r="AB7" s="76"/>
     </row>
@@ -34190,6 +34199,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P5:V5"/>
+    <mergeCell ref="V6:V7"/>
     <mergeCell ref="X6:X7"/>
     <mergeCell ref="W5:X5"/>
     <mergeCell ref="I2:Z2"/>
@@ -34206,18 +34227,6 @@
     <mergeCell ref="Y6:Y7"/>
     <mergeCell ref="Z6:Z7"/>
     <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H5:O5"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P5:V5"/>
-    <mergeCell ref="V6:V7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -34259,28 +34268,28 @@
     <row r="2" spans="2:29" ht="33" customHeight="1">
       <c r="B2" s="11"/>
       <c r="C2" s="20"/>
-      <c r="D2" s="171" t="s">
+      <c r="D2" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="171"/>
-      <c r="H2" s="171"/>
-      <c r="I2" s="171" t="s">
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="172"/>
+      <c r="H2" s="172"/>
+      <c r="I2" s="172" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="171"/>
-      <c r="K2" s="171"/>
-      <c r="L2" s="171"/>
-      <c r="M2" s="171"/>
-      <c r="N2" s="171"/>
-      <c r="O2" s="171"/>
-      <c r="R2" s="172" t="s">
+      <c r="J2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
+      <c r="M2" s="172"/>
+      <c r="N2" s="172"/>
+      <c r="O2" s="172"/>
+      <c r="R2" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="173"/>
-      <c r="T2" s="173"/>
-      <c r="U2" s="174"/>
+      <c r="S2" s="174"/>
+      <c r="T2" s="174"/>
+      <c r="U2" s="175"/>
     </row>
     <row r="4" spans="2:29" ht="15" customHeight="1">
       <c r="C4" s="21" t="s">
@@ -41546,32 +41555,32 @@
     </row>
     <row r="2" spans="1:27" ht="33" customHeight="1">
       <c r="A2" s="41"/>
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
       <c r="G2" s="59"/>
-      <c r="H2" s="176" t="s">
+      <c r="H2" s="178" t="s">
         <v>166</v>
       </c>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="178"/>
       <c r="N2" s="59"/>
       <c r="O2" s="59"/>
       <c r="P2" s="59"/>
       <c r="Q2" s="59"/>
       <c r="R2" s="89"/>
       <c r="S2" s="89"/>
-      <c r="T2" s="178" t="s">
+      <c r="T2" s="184" t="s">
         <v>167</v>
       </c>
-      <c r="U2" s="179"/>
+      <c r="U2" s="185"/>
       <c r="V2" s="41"/>
       <c r="W2" s="41"/>
       <c r="X2" s="41"/>
@@ -41633,7 +41642,7 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" thickTop="1">
       <c r="A5" s="41"/>
-      <c r="B5" s="183" t="s">
+      <c r="B5" s="187" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="180" t="s">
@@ -41667,56 +41676,56 @@
       <c r="U5" s="180" t="s">
         <v>120</v>
       </c>
-      <c r="V5" s="181"/>
+      <c r="V5" s="186"/>
       <c r="W5" s="41"/>
       <c r="X5" s="41"/>
       <c r="Y5" s="41"/>
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="41"/>
-      <c r="B6" s="184"/>
-      <c r="C6" s="182"/>
-      <c r="D6" s="182" t="s">
+      <c r="B6" s="188"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="181" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="182" t="s">
+      <c r="E6" s="181" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="182" t="s">
+      <c r="F6" s="181" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="182" t="s">
+      <c r="G6" s="181" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="182" t="s">
+      <c r="H6" s="181" t="s">
         <v>110</v>
       </c>
-      <c r="I6" s="182"/>
-      <c r="J6" s="182" t="s">
+      <c r="I6" s="181"/>
+      <c r="J6" s="181" t="s">
         <v>111</v>
       </c>
-      <c r="K6" s="182"/>
+      <c r="K6" s="181"/>
       <c r="L6" s="84" t="s">
         <v>112</v>
       </c>
-      <c r="M6" s="182" t="s">
+      <c r="M6" s="181" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="182"/>
-      <c r="O6" s="182"/>
-      <c r="P6" s="182" t="s">
+      <c r="N6" s="181"/>
+      <c r="O6" s="181"/>
+      <c r="P6" s="181" t="s">
         <v>117</v>
       </c>
-      <c r="Q6" s="182"/>
-      <c r="R6" s="182"/>
-      <c r="S6" s="182" t="s">
+      <c r="Q6" s="181"/>
+      <c r="R6" s="181"/>
+      <c r="S6" s="181" t="s">
         <v>112</v>
       </c>
-      <c r="T6" s="182"/>
-      <c r="U6" s="182" t="s">
+      <c r="T6" s="181"/>
+      <c r="U6" s="181" t="s">
         <v>121</v>
       </c>
-      <c r="V6" s="175" t="s">
+      <c r="V6" s="182" t="s">
         <v>122</v>
       </c>
       <c r="W6" s="41"/>
@@ -41725,12 +41734,12 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="41"/>
-      <c r="B7" s="184"/>
-      <c r="C7" s="182"/>
-      <c r="D7" s="182"/>
-      <c r="E7" s="182"/>
-      <c r="F7" s="182"/>
-      <c r="G7" s="182"/>
+      <c r="B7" s="188"/>
+      <c r="C7" s="181"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="181"/>
       <c r="H7" s="84" t="s">
         <v>108</v>
       </c>
@@ -41764,10 +41773,10 @@
       <c r="R7" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="182"/>
-      <c r="T7" s="182"/>
-      <c r="U7" s="182"/>
-      <c r="V7" s="175"/>
+      <c r="S7" s="181"/>
+      <c r="T7" s="181"/>
+      <c r="U7" s="181"/>
+      <c r="V7" s="182"/>
       <c r="W7" s="41"/>
       <c r="X7" s="41"/>
       <c r="Y7" s="41"/>
@@ -49276,11 +49285,11 @@
       <c r="P103" s="41"/>
       <c r="Q103" s="41"/>
       <c r="R103" s="41"/>
-      <c r="S103" s="185" t="s">
+      <c r="S103" s="176" t="s">
         <v>318</v>
       </c>
-      <c r="T103" s="185"/>
-      <c r="U103" s="185"/>
+      <c r="T103" s="176"/>
+      <c r="U103" s="176"/>
       <c r="V103" s="41"/>
       <c r="W103" s="41"/>
       <c r="X103" s="41"/>
@@ -49289,31 +49298,31 @@
     <row r="104" spans="1:27" s="5" customFormat="1" ht="63" customHeight="1">
       <c r="A104" s="91"/>
       <c r="B104" s="85"/>
-      <c r="C104" s="186" t="s">
+      <c r="C104" s="177" t="s">
         <v>308</v>
       </c>
-      <c r="D104" s="186"/>
+      <c r="D104" s="177"/>
       <c r="E104" s="91"/>
       <c r="F104" s="91"/>
       <c r="G104" s="91"/>
       <c r="H104" s="91"/>
       <c r="I104" s="91"/>
       <c r="J104" s="91"/>
-      <c r="K104" s="186" t="s">
+      <c r="K104" s="177" t="s">
         <v>309</v>
       </c>
-      <c r="L104" s="186"/>
-      <c r="M104" s="186"/>
+      <c r="L104" s="177"/>
+      <c r="M104" s="177"/>
       <c r="N104" s="91"/>
       <c r="O104" s="91"/>
       <c r="P104" s="91"/>
       <c r="Q104" s="91"/>
       <c r="R104" s="91"/>
-      <c r="S104" s="187" t="s">
+      <c r="S104" s="179" t="s">
         <v>339</v>
       </c>
-      <c r="T104" s="187"/>
-      <c r="U104" s="187"/>
+      <c r="T104" s="179"/>
+      <c r="U104" s="179"/>
       <c r="V104" s="91"/>
       <c r="W104" s="91"/>
       <c r="X104" s="91"/>
@@ -49405,31 +49414,31 @@
     <row r="108" spans="1:27" s="5" customFormat="1">
       <c r="A108" s="91"/>
       <c r="B108" s="85"/>
-      <c r="C108" s="186" t="s">
+      <c r="C108" s="177" t="s">
         <v>312</v>
       </c>
-      <c r="D108" s="186"/>
+      <c r="D108" s="177"/>
       <c r="E108" s="91"/>
       <c r="F108" s="91"/>
       <c r="G108" s="91"/>
       <c r="H108" s="91"/>
       <c r="I108" s="91"/>
       <c r="J108" s="91"/>
-      <c r="K108" s="186" t="s">
+      <c r="K108" s="177" t="s">
         <v>313</v>
       </c>
-      <c r="L108" s="186"/>
-      <c r="M108" s="186"/>
+      <c r="L108" s="177"/>
+      <c r="M108" s="177"/>
       <c r="N108" s="91"/>
       <c r="O108" s="91"/>
       <c r="P108" s="91"/>
       <c r="Q108" s="91"/>
       <c r="R108" s="91"/>
-      <c r="S108" s="186" t="s">
+      <c r="S108" s="177" t="s">
         <v>314</v>
       </c>
-      <c r="T108" s="186"/>
-      <c r="U108" s="186"/>
+      <c r="T108" s="177"/>
+      <c r="U108" s="177"/>
       <c r="V108" s="91"/>
       <c r="W108" s="91"/>
       <c r="X108" s="91"/>
@@ -49790,6 +49799,20 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="B5:B7"/>
     <mergeCell ref="S103:U103"/>
     <mergeCell ref="S108:U108"/>
     <mergeCell ref="H2:M2"/>
@@ -49804,20 +49827,6 @@
     <mergeCell ref="M5:S5"/>
     <mergeCell ref="T5:T7"/>
     <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" orientation="landscape" r:id="rId1"/>
@@ -49852,117 +49861,117 @@
         <v>125</v>
       </c>
       <c r="S2" s="35"/>
-      <c r="AA2" s="189" t="s">
+      <c r="AA2" s="190" t="s">
         <v>143</v>
       </c>
-      <c r="AB2" s="190"/>
+      <c r="AB2" s="191"/>
     </row>
     <row r="5" spans="2:30">
-      <c r="B5" s="188" t="s">
+      <c r="B5" s="189" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
-      <c r="E5" s="188" t="s">
+      <c r="E5" s="189" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="188" t="s">
+      <c r="F5" s="189" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="188"/>
-      <c r="H5" s="188"/>
-      <c r="I5" s="188"/>
-      <c r="J5" s="188" t="s">
+      <c r="G5" s="189"/>
+      <c r="H5" s="189"/>
+      <c r="I5" s="189"/>
+      <c r="J5" s="189" t="s">
         <v>131</v>
       </c>
-      <c r="K5" s="188"/>
-      <c r="L5" s="188"/>
-      <c r="M5" s="188" t="s">
+      <c r="K5" s="189"/>
+      <c r="L5" s="189"/>
+      <c r="M5" s="189" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="188"/>
-      <c r="O5" s="188"/>
-      <c r="P5" s="188" t="s">
+      <c r="N5" s="189"/>
+      <c r="O5" s="189"/>
+      <c r="P5" s="189" t="s">
         <v>134</v>
       </c>
-      <c r="Q5" s="188" t="s">
+      <c r="Q5" s="189" t="s">
         <v>135</v>
       </c>
-      <c r="R5" s="188" t="s">
+      <c r="R5" s="189" t="s">
         <v>136</v>
       </c>
-      <c r="S5" s="188"/>
-      <c r="T5" s="188"/>
-      <c r="U5" s="188"/>
-      <c r="V5" s="188" t="s">
+      <c r="S5" s="189"/>
+      <c r="T5" s="189"/>
+      <c r="U5" s="189"/>
+      <c r="V5" s="189" t="s">
         <v>138</v>
       </c>
-      <c r="W5" s="188"/>
-      <c r="X5" s="188" t="s">
+      <c r="W5" s="189"/>
+      <c r="X5" s="189" t="s">
         <v>139</v>
       </c>
-      <c r="Y5" s="188"/>
-      <c r="Z5" s="188" t="s">
+      <c r="Y5" s="189"/>
+      <c r="Z5" s="189" t="s">
         <v>140</v>
       </c>
-      <c r="AA5" s="188"/>
-      <c r="AB5" s="188"/>
-      <c r="AC5" s="188"/>
-      <c r="AD5" s="188" t="s">
+      <c r="AA5" s="189"/>
+      <c r="AB5" s="189"/>
+      <c r="AC5" s="189"/>
+      <c r="AD5" s="189" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:30">
-      <c r="B6" s="188"/>
+      <c r="B6" s="189"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
-      <c r="E6" s="188"/>
-      <c r="F6" s="188" t="s">
+      <c r="E6" s="189"/>
+      <c r="F6" s="189" t="s">
         <v>128</v>
       </c>
-      <c r="G6" s="188"/>
-      <c r="H6" s="188"/>
-      <c r="I6" s="188" t="s">
+      <c r="G6" s="189"/>
+      <c r="H6" s="189"/>
+      <c r="I6" s="189" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="188" t="s">
+      <c r="J6" s="189" t="s">
         <v>212</v>
       </c>
-      <c r="K6" s="188" t="s">
+      <c r="K6" s="189" t="s">
         <v>129</v>
       </c>
-      <c r="L6" s="188" t="s">
+      <c r="L6" s="189" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="188" t="s">
+      <c r="M6" s="189" t="s">
         <v>132</v>
       </c>
-      <c r="N6" s="188" t="s">
+      <c r="N6" s="189" t="s">
         <v>133</v>
       </c>
-      <c r="O6" s="188" t="s">
+      <c r="O6" s="189" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="188"/>
-      <c r="Q6" s="188"/>
-      <c r="R6" s="188" t="s">
+      <c r="P6" s="189"/>
+      <c r="Q6" s="189"/>
+      <c r="R6" s="189" t="s">
         <v>128</v>
       </c>
-      <c r="S6" s="188"/>
-      <c r="T6" s="188" t="s">
+      <c r="S6" s="189"/>
+      <c r="T6" s="189" t="s">
         <v>137</v>
       </c>
-      <c r="U6" s="188"/>
-      <c r="V6" s="188" t="s">
+      <c r="U6" s="189"/>
+      <c r="V6" s="189" t="s">
         <v>129</v>
       </c>
-      <c r="W6" s="188" t="s">
+      <c r="W6" s="189" t="s">
         <v>130</v>
       </c>
-      <c r="X6" s="188" t="s">
+      <c r="X6" s="189" t="s">
         <v>129</v>
       </c>
-      <c r="Y6" s="188" t="s">
+      <c r="Y6" s="189" t="s">
         <v>130</v>
       </c>
       <c r="Z6" s="33" t="s">
@@ -49973,13 +49982,13 @@
         <v>133</v>
       </c>
       <c r="AC6" s="33"/>
-      <c r="AD6" s="188"/>
+      <c r="AD6" s="189"/>
     </row>
     <row r="7" spans="2:30">
-      <c r="B7" s="188"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
-      <c r="E7" s="188"/>
+      <c r="E7" s="189"/>
       <c r="F7" s="33" t="s">
         <v>212</v>
       </c>
@@ -49989,15 +49998,15 @@
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="188"/>
-      <c r="J7" s="188"/>
-      <c r="K7" s="188"/>
-      <c r="L7" s="188"/>
-      <c r="M7" s="188"/>
-      <c r="N7" s="188"/>
-      <c r="O7" s="188"/>
-      <c r="P7" s="188"/>
-      <c r="Q7" s="188"/>
+      <c r="I7" s="189"/>
+      <c r="J7" s="189"/>
+      <c r="K7" s="189"/>
+      <c r="L7" s="189"/>
+      <c r="M7" s="189"/>
+      <c r="N7" s="189"/>
+      <c r="O7" s="189"/>
+      <c r="P7" s="189"/>
+      <c r="Q7" s="189"/>
       <c r="R7" s="33" t="s">
         <v>121</v>
       </c>
@@ -50010,10 +50019,10 @@
       <c r="U7" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="V7" s="188"/>
-      <c r="W7" s="188"/>
-      <c r="X7" s="188"/>
-      <c r="Y7" s="188"/>
+      <c r="V7" s="189"/>
+      <c r="W7" s="189"/>
+      <c r="X7" s="189"/>
+      <c r="Y7" s="189"/>
       <c r="Z7" s="33" t="s">
         <v>122</v>
       </c>
@@ -50026,7 +50035,7 @@
       <c r="AC7" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="AD7" s="188"/>
+      <c r="AD7" s="189"/>
     </row>
     <row r="9" spans="2:30" s="5" customFormat="1">
       <c r="B9" s="5" t="s">
@@ -62453,6 +62462,24 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="Q5:Q7"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
     <mergeCell ref="AD5:AD7"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="W6:W7"/>
@@ -62462,24 +62489,6 @@
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="Z5:AC5"/>
     <mergeCell ref="V6:V7"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="Q5:Q7"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="I6:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -62507,34 +62516,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:28" s="44" customFormat="1" ht="35.25" customHeight="1">
-      <c r="B2" s="203" t="s">
+      <c r="B2" s="201" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="203"/>
-      <c r="D2" s="203"/>
-      <c r="E2" s="203"/>
-      <c r="F2" s="203"/>
-      <c r="G2" s="203"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="202" t="s">
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="201"/>
+      <c r="F2" s="201"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="200" t="s">
         <v>164</v>
       </c>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
-      <c r="M2" s="202"/>
-      <c r="N2" s="202"/>
-      <c r="O2" s="202"/>
-      <c r="P2" s="202"/>
-      <c r="Q2" s="202"/>
-      <c r="R2" s="202"/>
-      <c r="S2" s="202"/>
+      <c r="J2" s="200"/>
+      <c r="K2" s="200"/>
+      <c r="L2" s="200"/>
+      <c r="M2" s="200"/>
+      <c r="N2" s="200"/>
+      <c r="O2" s="200"/>
+      <c r="P2" s="200"/>
+      <c r="Q2" s="200"/>
+      <c r="R2" s="200"/>
+      <c r="S2" s="200"/>
       <c r="T2" s="43"/>
       <c r="U2" s="43"/>
-      <c r="Y2" s="196" t="s">
+      <c r="Y2" s="192" t="s">
         <v>143</v>
       </c>
-      <c r="Z2" s="197"/>
+      <c r="Z2" s="193"/>
     </row>
     <row r="3" spans="2:28">
       <c r="Q3" s="37"/>
@@ -62569,107 +62578,107 @@
       <c r="AB4" s="7"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" thickTop="1">
-      <c r="B5" s="198" t="s">
+      <c r="B5" s="194" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="200" t="s">
+      <c r="C5" s="196" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="200" t="s">
+      <c r="D5" s="196" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="200"/>
-      <c r="F5" s="200"/>
-      <c r="G5" s="200"/>
-      <c r="H5" s="200" t="s">
+      <c r="E5" s="196"/>
+      <c r="F5" s="196"/>
+      <c r="G5" s="196"/>
+      <c r="H5" s="196" t="s">
         <v>131</v>
       </c>
-      <c r="I5" s="200"/>
-      <c r="J5" s="200"/>
-      <c r="K5" s="200" t="s">
+      <c r="I5" s="196"/>
+      <c r="J5" s="196"/>
+      <c r="K5" s="196" t="s">
         <v>113</v>
       </c>
-      <c r="L5" s="200"/>
-      <c r="M5" s="200"/>
-      <c r="N5" s="201" t="s">
+      <c r="L5" s="196"/>
+      <c r="M5" s="196"/>
+      <c r="N5" s="198" t="s">
         <v>134</v>
       </c>
-      <c r="O5" s="201" t="s">
+      <c r="O5" s="198" t="s">
         <v>135</v>
       </c>
-      <c r="P5" s="200" t="s">
+      <c r="P5" s="196" t="s">
         <v>136</v>
       </c>
-      <c r="Q5" s="200"/>
-      <c r="R5" s="200"/>
-      <c r="S5" s="200"/>
-      <c r="T5" s="201" t="s">
+      <c r="Q5" s="196"/>
+      <c r="R5" s="196"/>
+      <c r="S5" s="196"/>
+      <c r="T5" s="198" t="s">
         <v>138</v>
       </c>
-      <c r="U5" s="201"/>
-      <c r="V5" s="200" t="s">
+      <c r="U5" s="198"/>
+      <c r="V5" s="196" t="s">
         <v>139</v>
       </c>
-      <c r="W5" s="200"/>
-      <c r="X5" s="200" t="s">
+      <c r="W5" s="196"/>
+      <c r="X5" s="196" t="s">
         <v>140</v>
       </c>
-      <c r="Y5" s="200"/>
-      <c r="Z5" s="200"/>
-      <c r="AA5" s="200"/>
-      <c r="AB5" s="192" t="s">
+      <c r="Y5" s="196"/>
+      <c r="Z5" s="196"/>
+      <c r="AA5" s="196"/>
+      <c r="AB5" s="203" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:28">
-      <c r="B6" s="199"/>
-      <c r="C6" s="194"/>
-      <c r="D6" s="194" t="s">
+      <c r="B6" s="195"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197" t="s">
         <v>128</v>
       </c>
-      <c r="E6" s="194"/>
-      <c r="F6" s="194"/>
-      <c r="G6" s="195" t="s">
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="199" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="194" t="s">
+      <c r="H6" s="197" t="s">
         <v>133</v>
       </c>
-      <c r="I6" s="194" t="s">
+      <c r="I6" s="197" t="s">
         <v>132</v>
       </c>
-      <c r="J6" s="194" t="s">
+      <c r="J6" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="195" t="s">
+      <c r="K6" s="199" t="s">
         <v>133</v>
       </c>
-      <c r="L6" s="195" t="s">
+      <c r="L6" s="199" t="s">
         <v>132</v>
       </c>
-      <c r="M6" s="195" t="s">
+      <c r="M6" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="195"/>
-      <c r="O6" s="195"/>
-      <c r="P6" s="194" t="s">
+      <c r="N6" s="199"/>
+      <c r="O6" s="199"/>
+      <c r="P6" s="197" t="s">
         <v>128</v>
       </c>
-      <c r="Q6" s="194"/>
-      <c r="R6" s="194" t="s">
+      <c r="Q6" s="197"/>
+      <c r="R6" s="197" t="s">
         <v>137</v>
       </c>
-      <c r="S6" s="194"/>
-      <c r="T6" s="195" t="s">
+      <c r="S6" s="197"/>
+      <c r="T6" s="199" t="s">
         <v>129</v>
       </c>
-      <c r="U6" s="195" t="s">
+      <c r="U6" s="199" t="s">
         <v>130</v>
       </c>
-      <c r="V6" s="194" t="s">
+      <c r="V6" s="197" t="s">
         <v>129</v>
       </c>
-      <c r="W6" s="194" t="s">
+      <c r="W6" s="197" t="s">
         <v>130</v>
       </c>
       <c r="X6" s="2" t="s">
@@ -62680,11 +62689,11 @@
         <v>133</v>
       </c>
       <c r="AA6" s="2"/>
-      <c r="AB6" s="193"/>
+      <c r="AB6" s="204"/>
     </row>
     <row r="7" spans="2:28">
-      <c r="B7" s="199"/>
-      <c r="C7" s="194"/>
+      <c r="B7" s="195"/>
+      <c r="C7" s="197"/>
       <c r="D7" s="2" t="s">
         <v>129</v>
       </c>
@@ -62694,15 +62703,15 @@
       <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="195"/>
-      <c r="H7" s="194"/>
-      <c r="I7" s="194"/>
-      <c r="J7" s="194"/>
-      <c r="K7" s="195"/>
-      <c r="L7" s="195"/>
-      <c r="M7" s="195"/>
-      <c r="N7" s="195"/>
-      <c r="O7" s="195"/>
+      <c r="G7" s="199"/>
+      <c r="H7" s="197"/>
+      <c r="I7" s="197"/>
+      <c r="J7" s="197"/>
+      <c r="K7" s="199"/>
+      <c r="L7" s="199"/>
+      <c r="M7" s="199"/>
+      <c r="N7" s="199"/>
+      <c r="O7" s="199"/>
       <c r="P7" s="2" t="s">
         <v>121</v>
       </c>
@@ -62715,10 +62724,10 @@
       <c r="S7" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="T7" s="195"/>
-      <c r="U7" s="195"/>
-      <c r="V7" s="194"/>
-      <c r="W7" s="194"/>
+      <c r="T7" s="199"/>
+      <c r="U7" s="199"/>
+      <c r="V7" s="197"/>
+      <c r="W7" s="197"/>
       <c r="X7" s="2" t="s">
         <v>122</v>
       </c>
@@ -62731,7 +62740,7 @@
       <c r="AA7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AB7" s="193"/>
+      <c r="AB7" s="204"/>
     </row>
     <row r="8" spans="2:28" s="5" customFormat="1">
       <c r="B8" s="27" t="str">
@@ -76274,68 +76283,91 @@
       <c r="C193" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="F193" s="169" t="s">
+      <c r="F193" s="162" t="s">
         <v>463</v>
       </c>
-      <c r="G193" s="169"/>
-      <c r="J193" s="169" t="s">
+      <c r="G193" s="162"/>
+      <c r="J193" s="162" t="s">
         <v>465</v>
       </c>
-      <c r="K193" s="169"/>
-      <c r="L193" s="169"/>
+      <c r="K193" s="162"/>
+      <c r="L193" s="162"/>
       <c r="M193" s="115"/>
       <c r="N193" s="115"/>
-      <c r="O193" s="191" t="s">
+      <c r="O193" s="202" t="s">
         <v>467</v>
       </c>
-      <c r="P193" s="191"/>
-      <c r="Q193" s="191"/>
-      <c r="T193" s="191" t="s">
+      <c r="P193" s="202"/>
+      <c r="Q193" s="202"/>
+      <c r="T193" s="202" t="s">
         <v>469</v>
       </c>
-      <c r="U193" s="191"/>
-      <c r="V193" s="191"/>
-      <c r="Y193" s="169" t="s">
+      <c r="U193" s="202"/>
+      <c r="V193" s="202"/>
+      <c r="Y193" s="162" t="s">
         <v>471</v>
       </c>
-      <c r="Z193" s="169"/>
-      <c r="AA193" s="169"/>
+      <c r="Z193" s="162"/>
+      <c r="AA193" s="162"/>
     </row>
     <row r="197" spans="2:27" s="5" customFormat="1">
       <c r="B197" s="114"/>
       <c r="C197" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="F197" s="169" t="s">
+      <c r="F197" s="162" t="s">
         <v>464</v>
       </c>
-      <c r="G197" s="169"/>
+      <c r="G197" s="162"/>
       <c r="H197" s="66"/>
-      <c r="J197" s="169" t="s">
+      <c r="J197" s="162" t="s">
         <v>466</v>
       </c>
-      <c r="K197" s="169"/>
-      <c r="L197" s="169"/>
+      <c r="K197" s="162"/>
+      <c r="L197" s="162"/>
       <c r="M197" s="115"/>
       <c r="N197" s="115"/>
-      <c r="O197" s="191" t="s">
+      <c r="O197" s="202" t="s">
         <v>468</v>
       </c>
-      <c r="P197" s="191"/>
-      <c r="Q197" s="191"/>
-      <c r="T197" s="191" t="s">
+      <c r="P197" s="202"/>
+      <c r="Q197" s="202"/>
+      <c r="T197" s="202" t="s">
         <v>470</v>
       </c>
-      <c r="U197" s="191"/>
-      <c r="V197" s="191"/>
-      <c r="Y197" s="169" t="s">
+      <c r="U197" s="202"/>
+      <c r="V197" s="202"/>
+      <c r="Y197" s="162" t="s">
         <v>472</v>
       </c>
-      <c r="Z197" s="169"/>
-      <c r="AA197" s="169"/>
+      <c r="Z197" s="162"/>
+      <c r="AA197" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="T197:V197"/>
+    <mergeCell ref="T193:V193"/>
+    <mergeCell ref="Y197:AA197"/>
+    <mergeCell ref="Y193:AA193"/>
+    <mergeCell ref="AB5:AB7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="F193:G193"/>
+    <mergeCell ref="F197:G197"/>
+    <mergeCell ref="J197:L197"/>
+    <mergeCell ref="J193:L193"/>
+    <mergeCell ref="O193:Q193"/>
+    <mergeCell ref="O197:Q197"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
@@ -76352,29 +76384,6 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
-    <mergeCell ref="F193:G193"/>
-    <mergeCell ref="F197:G197"/>
-    <mergeCell ref="J197:L197"/>
-    <mergeCell ref="J193:L193"/>
-    <mergeCell ref="O193:Q193"/>
-    <mergeCell ref="O197:Q197"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="T197:V197"/>
-    <mergeCell ref="T193:V193"/>
-    <mergeCell ref="Y197:AA197"/>
-    <mergeCell ref="Y193:AA193"/>
-    <mergeCell ref="AB5:AB7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="V6:V7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -76409,10 +76418,10 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="204" t="s">
+      <c r="L6" s="205" t="s">
         <v>280</v>
       </c>
-      <c r="M6" s="204"/>
+      <c r="M6" s="205"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -82067,19 +82076,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="29.25" customHeight="1">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="203" t="s">
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="201" t="s">
         <v>282</v>
       </c>
-      <c r="F2" s="203"/>
-      <c r="G2" s="203"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="203"/>
-      <c r="J2" s="203"/>
+      <c r="F2" s="201"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="201"/>
+      <c r="J2" s="201"/>
       <c r="K2" s="116"/>
       <c r="L2" s="116"/>
       <c r="N2" s="78" t="s">
@@ -82087,86 +82096,86 @@
       </c>
     </row>
     <row r="4" spans="2:14" ht="15.75" thickBot="1">
-      <c r="K4" s="205" t="s">
+      <c r="K4" s="214" t="s">
         <v>473</v>
       </c>
-      <c r="L4" s="205"/>
-      <c r="M4" s="205"/>
+      <c r="L4" s="214"/>
+      <c r="M4" s="214"/>
     </row>
     <row r="5" spans="2:14" ht="15.75" thickTop="1">
-      <c r="B5" s="211" t="s">
+      <c r="B5" s="208" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="213" t="s">
+      <c r="C5" s="210" t="s">
         <v>262</v>
       </c>
-      <c r="D5" s="200" t="s">
+      <c r="D5" s="196" t="s">
         <v>263</v>
       </c>
-      <c r="E5" s="215" t="s">
+      <c r="E5" s="212" t="s">
         <v>264</v>
       </c>
-      <c r="F5" s="215"/>
-      <c r="G5" s="215" t="s">
+      <c r="F5" s="212"/>
+      <c r="G5" s="212" t="s">
         <v>267</v>
       </c>
-      <c r="H5" s="215"/>
-      <c r="I5" s="215"/>
-      <c r="J5" s="215"/>
-      <c r="K5" s="215" t="s">
+      <c r="H5" s="212"/>
+      <c r="I5" s="212"/>
+      <c r="J5" s="212"/>
+      <c r="K5" s="212" t="s">
         <v>272</v>
       </c>
-      <c r="L5" s="215"/>
-      <c r="M5" s="215"/>
-      <c r="N5" s="216"/>
+      <c r="L5" s="212"/>
+      <c r="M5" s="212"/>
+      <c r="N5" s="213"/>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="212"/>
-      <c r="C6" s="214"/>
-      <c r="D6" s="194"/>
-      <c r="E6" s="209" t="s">
+      <c r="B6" s="209"/>
+      <c r="C6" s="211"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="206" t="s">
         <v>265</v>
       </c>
-      <c r="F6" s="209" t="s">
+      <c r="F6" s="206" t="s">
         <v>266</v>
       </c>
-      <c r="G6" s="209" t="s">
+      <c r="G6" s="206" t="s">
         <v>268</v>
       </c>
-      <c r="H6" s="209" t="s">
+      <c r="H6" s="206" t="s">
         <v>269</v>
       </c>
-      <c r="I6" s="209" t="s">
+      <c r="I6" s="206" t="s">
         <v>270</v>
       </c>
-      <c r="J6" s="209"/>
-      <c r="K6" s="209" t="s">
+      <c r="J6" s="206"/>
+      <c r="K6" s="206" t="s">
         <v>273</v>
       </c>
-      <c r="L6" s="209" t="s">
+      <c r="L6" s="206" t="s">
         <v>269</v>
       </c>
-      <c r="M6" s="209" t="s">
+      <c r="M6" s="206" t="s">
         <v>270</v>
       </c>
-      <c r="N6" s="210"/>
+      <c r="N6" s="207"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="212"/>
-      <c r="C7" s="214"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="209"/>
-      <c r="H7" s="209"/>
+      <c r="B7" s="209"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="197"/>
+      <c r="E7" s="206"/>
+      <c r="F7" s="206"/>
+      <c r="G7" s="206"/>
+      <c r="H7" s="206"/>
       <c r="I7" s="86" t="s">
         <v>271</v>
       </c>
       <c r="J7" s="86" t="s">
         <v>141</v>
       </c>
-      <c r="K7" s="209"/>
-      <c r="L7" s="209"/>
+      <c r="K7" s="206"/>
+      <c r="L7" s="206"/>
       <c r="M7" s="86" t="s">
         <v>122</v>
       </c>
@@ -87918,11 +87927,11 @@
       <c r="H155" s="10"/>
       <c r="I155" s="10"/>
       <c r="J155" s="10"/>
-      <c r="K155" s="208" t="s">
+      <c r="K155" s="217" t="s">
         <v>318</v>
       </c>
-      <c r="L155" s="208"/>
-      <c r="M155" s="208"/>
+      <c r="L155" s="217"/>
+      <c r="M155" s="217"/>
       <c r="N155" s="10"/>
     </row>
     <row r="156" spans="1:14" s="21" customFormat="1" ht="74.25" customHeight="1">
@@ -87932,15 +87941,15 @@
       <c r="D156" s="22"/>
       <c r="E156" s="22"/>
       <c r="F156" s="22"/>
-      <c r="G156" s="206"/>
-      <c r="H156" s="206"/>
-      <c r="I156" s="206"/>
+      <c r="G156" s="215"/>
+      <c r="H156" s="215"/>
+      <c r="I156" s="215"/>
       <c r="J156" s="22"/>
-      <c r="K156" s="207" t="s">
+      <c r="K156" s="216" t="s">
         <v>311</v>
       </c>
-      <c r="L156" s="207"/>
-      <c r="M156" s="207"/>
+      <c r="L156" s="216"/>
+      <c r="M156" s="216"/>
       <c r="N156" s="22"/>
     </row>
     <row r="157" spans="1:14" s="21" customFormat="1" ht="14.25">
@@ -87952,11 +87961,11 @@
       <c r="D157" s="22"/>
       <c r="E157" s="22"/>
       <c r="F157" s="22"/>
-      <c r="G157" s="206" t="s">
+      <c r="G157" s="215" t="s">
         <v>309</v>
       </c>
-      <c r="H157" s="206"/>
-      <c r="I157" s="206"/>
+      <c r="H157" s="215"/>
+      <c r="I157" s="215"/>
       <c r="J157" s="22"/>
       <c r="K157" s="22"/>
       <c r="L157" s="22"/>
@@ -88020,17 +88029,17 @@
       <c r="D161" s="22"/>
       <c r="E161" s="22"/>
       <c r="F161" s="22"/>
-      <c r="G161" s="206" t="s">
+      <c r="G161" s="215" t="s">
         <v>313</v>
       </c>
-      <c r="H161" s="206"/>
-      <c r="I161" s="206"/>
+      <c r="H161" s="215"/>
+      <c r="I161" s="215"/>
       <c r="J161" s="22"/>
-      <c r="K161" s="206" t="s">
+      <c r="K161" s="215" t="s">
         <v>314</v>
       </c>
-      <c r="L161" s="206"/>
-      <c r="M161" s="206"/>
+      <c r="L161" s="215"/>
+      <c r="M161" s="215"/>
       <c r="N161" s="10"/>
     </row>
     <row r="162" spans="1:14">
@@ -88643,6 +88652,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="G156:I156"/>
+    <mergeCell ref="G161:I161"/>
+    <mergeCell ref="K156:M156"/>
+    <mergeCell ref="G157:I157"/>
+    <mergeCell ref="K155:M155"/>
+    <mergeCell ref="K161:M161"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="I6:J6"/>
@@ -88659,13 +88675,6 @@
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="E2:J2"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="G156:I156"/>
-    <mergeCell ref="G161:I161"/>
-    <mergeCell ref="K156:M156"/>
-    <mergeCell ref="G157:I157"/>
-    <mergeCell ref="K155:M155"/>
-    <mergeCell ref="K161:M161"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>